<commit_message>
nw acc delay unlinked from excel
</commit_message>
<xml_diff>
--- a/stakeholder_lists.xlsx
+++ b/stakeholder_lists.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\mobile-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46AD1D2B-4D3D-4BFF-9534-C01835D6BC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D921B456-CA09-4899-88FF-41DCD2DDF33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{17D0CF8C-6239-4396-93EE-ED3916C7EA4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="1" xr2:uid="{17D0CF8C-6239-4396-93EE-ED3916C7EA4B}"/>
   </bookViews>
   <sheets>
     <sheet name="state_lists" sheetId="1" r:id="rId1"/>
+    <sheet name="acc_lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="417">
   <si>
     <t>state</t>
   </si>
@@ -636,13 +637,664 @@
   </si>
   <si>
     <t>EG</t>
+  </si>
+  <si>
+    <t>NM_name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ICAO_code</t>
+  </si>
+  <si>
+    <t>AGADIR ACC</t>
+  </si>
+  <si>
+    <t>Agadir ACC</t>
+  </si>
+  <si>
+    <t>GMACACC</t>
+  </si>
+  <si>
+    <t>AMSTERDAM ACC</t>
+  </si>
+  <si>
+    <t>Amsterdam ACC</t>
+  </si>
+  <si>
+    <t>EHAAACC</t>
+  </si>
+  <si>
+    <t>ANKARA ACC</t>
+  </si>
+  <si>
+    <t>Ankara ACC</t>
+  </si>
+  <si>
+    <t>LTAAACC</t>
+  </si>
+  <si>
+    <t>ATHINAI ACC</t>
+  </si>
+  <si>
+    <t>Athens ACC</t>
+  </si>
+  <si>
+    <t>LGGGACC</t>
+  </si>
+  <si>
+    <t>BARCELONA ACC</t>
+  </si>
+  <si>
+    <t>Barcelona ACC</t>
+  </si>
+  <si>
+    <t>LECBACC</t>
+  </si>
+  <si>
+    <t>BEOGRAD ACC</t>
+  </si>
+  <si>
+    <t>Belgrade ACC</t>
+  </si>
+  <si>
+    <t>LYBAACC</t>
+  </si>
+  <si>
+    <t>BODO ACC</t>
+  </si>
+  <si>
+    <t>Bodo ACC</t>
+  </si>
+  <si>
+    <t>ENBDACC</t>
+  </si>
+  <si>
+    <t>BORDEAUX ACC</t>
+  </si>
+  <si>
+    <t>Bordeaux ACC</t>
+  </si>
+  <si>
+    <t>LFBBALL</t>
+  </si>
+  <si>
+    <t>BRATISLAVA ACC</t>
+  </si>
+  <si>
+    <t>Bratislava ACC</t>
+  </si>
+  <si>
+    <t>LZBBACC</t>
+  </si>
+  <si>
+    <t>BREMEN ACC</t>
+  </si>
+  <si>
+    <t>Bremen ACC</t>
+  </si>
+  <si>
+    <t>EDWWACC</t>
+  </si>
+  <si>
+    <t>BREST ACC</t>
+  </si>
+  <si>
+    <t>Brest ACC</t>
+  </si>
+  <si>
+    <t>LFRRACC</t>
+  </si>
+  <si>
+    <t>BRINDISI ACC</t>
+  </si>
+  <si>
+    <t>Brindisi ACC</t>
+  </si>
+  <si>
+    <t>LIBBACC</t>
+  </si>
+  <si>
+    <t>BRUSSELS ACC</t>
+  </si>
+  <si>
+    <t>Brussels ACC</t>
+  </si>
+  <si>
+    <t>EBBUACC</t>
+  </si>
+  <si>
+    <t>BUCURESTI ACC</t>
+  </si>
+  <si>
+    <t>Bucharest ACC</t>
+  </si>
+  <si>
+    <t>LRBBACC</t>
+  </si>
+  <si>
+    <t>BUDAPEST ACC</t>
+  </si>
+  <si>
+    <t>Budapest ACC</t>
+  </si>
+  <si>
+    <t>LHCCACC</t>
+  </si>
+  <si>
+    <t>CANARIAS ACC</t>
+  </si>
+  <si>
+    <t>Canaries ACC</t>
+  </si>
+  <si>
+    <t>GCCCACC</t>
+  </si>
+  <si>
+    <t>CASABLANCA ACC</t>
+  </si>
+  <si>
+    <t>Casablanca ACC</t>
+  </si>
+  <si>
+    <t>GMMMACC</t>
+  </si>
+  <si>
+    <t>CHISINAU ACC</t>
+  </si>
+  <si>
+    <t>Chisinau ACC</t>
+  </si>
+  <si>
+    <t>LUUUACC</t>
+  </si>
+  <si>
+    <t>DNIPRO ACC</t>
+  </si>
+  <si>
+    <t>Dnipro ACC</t>
+  </si>
+  <si>
+    <t>UKDVACC</t>
+  </si>
+  <si>
+    <t>DUBLIN ACC</t>
+  </si>
+  <si>
+    <t>Dublin ACC</t>
+  </si>
+  <si>
+    <t>EIDWACC</t>
+  </si>
+  <si>
+    <t>GENEVA ACC</t>
+  </si>
+  <si>
+    <t>Geneva ACC</t>
+  </si>
+  <si>
+    <t>LSAGACC</t>
+  </si>
+  <si>
+    <t>HELSINKI ACC</t>
+  </si>
+  <si>
+    <t>Helsinki ACC</t>
+  </si>
+  <si>
+    <t>EFINACC</t>
+  </si>
+  <si>
+    <t>ISTANBUL ACC</t>
+  </si>
+  <si>
+    <t>Istanbul ACC</t>
+  </si>
+  <si>
+    <t>LTBBACC</t>
+  </si>
+  <si>
+    <t>KARLSRUHE ACC</t>
+  </si>
+  <si>
+    <t>Karlsruhe UAC</t>
+  </si>
+  <si>
+    <t>EDUUUAC</t>
+  </si>
+  <si>
+    <t>KOBENHAVN ACC</t>
+  </si>
+  <si>
+    <t>Copenhagen ACC</t>
+  </si>
+  <si>
+    <t>EKDKACC</t>
+  </si>
+  <si>
+    <t>KYIV ACC</t>
+  </si>
+  <si>
+    <t>Kyiv ACC</t>
+  </si>
+  <si>
+    <t>UKBVACC</t>
+  </si>
+  <si>
+    <t>LANGEN ACC</t>
+  </si>
+  <si>
+    <t>Langen ACC</t>
+  </si>
+  <si>
+    <t>EDGGALL</t>
+  </si>
+  <si>
+    <t>LISBOA ACC</t>
+  </si>
+  <si>
+    <t>Lisbon ACC</t>
+  </si>
+  <si>
+    <t>LPPCACC</t>
+  </si>
+  <si>
+    <t>LJUBLJANA ACC</t>
+  </si>
+  <si>
+    <t>Ljubljana ACC</t>
+  </si>
+  <si>
+    <t>LJLAACC</t>
+  </si>
+  <si>
+    <t>LONDON ACC</t>
+  </si>
+  <si>
+    <t>London ACC</t>
+  </si>
+  <si>
+    <t>EGTTACC</t>
+  </si>
+  <si>
+    <t>LONDON TMA TC</t>
+  </si>
+  <si>
+    <t>London TMA TC</t>
+  </si>
+  <si>
+    <t>EGTTTC</t>
+  </si>
+  <si>
+    <t>L'VIV ACC</t>
+  </si>
+  <si>
+    <t>L'viv ACC</t>
+  </si>
+  <si>
+    <t>UKLVACC</t>
+  </si>
+  <si>
+    <t>MAASTRICHT UAC</t>
+  </si>
+  <si>
+    <t>Maastricht UAC</t>
+  </si>
+  <si>
+    <t>MAS</t>
+  </si>
+  <si>
+    <t>EDYYUAC</t>
+  </si>
+  <si>
+    <t>MADRID ACC</t>
+  </si>
+  <si>
+    <t>Madrid ACC</t>
+  </si>
+  <si>
+    <t>LECMALL</t>
+  </si>
+  <si>
+    <t>MAKEDONIA ACC</t>
+  </si>
+  <si>
+    <t>Makedonia ACC</t>
+  </si>
+  <si>
+    <t>LGMDACC</t>
+  </si>
+  <si>
+    <t>MALMO ACC</t>
+  </si>
+  <si>
+    <t>Malmo ACC</t>
+  </si>
+  <si>
+    <t>ESMMACC</t>
+  </si>
+  <si>
+    <t>MALTA ACC</t>
+  </si>
+  <si>
+    <t>Malta ACC</t>
+  </si>
+  <si>
+    <t>LMMMACC</t>
+  </si>
+  <si>
+    <t>MARSEILLE ACC</t>
+  </si>
+  <si>
+    <t>Marseille ACC</t>
+  </si>
+  <si>
+    <t>LFMMACC</t>
+  </si>
+  <si>
+    <t>MILANO ACC</t>
+  </si>
+  <si>
+    <t>Milan ACC</t>
+  </si>
+  <si>
+    <t>LIMMACC</t>
+  </si>
+  <si>
+    <t>MUENCHEN ACC</t>
+  </si>
+  <si>
+    <t>Munich ACC</t>
+  </si>
+  <si>
+    <t>EDMMACC</t>
+  </si>
+  <si>
+    <t>NICOSIA ACC</t>
+  </si>
+  <si>
+    <t>Nicosia ACC</t>
+  </si>
+  <si>
+    <t>LCCCACC</t>
+  </si>
+  <si>
+    <t>ODESA ACC</t>
+  </si>
+  <si>
+    <t>Odesa ACC</t>
+  </si>
+  <si>
+    <t>UKOVACC</t>
+  </si>
+  <si>
+    <t>OSLO ACC</t>
+  </si>
+  <si>
+    <t>Oslo ACC</t>
+  </si>
+  <si>
+    <t>ENOSACC</t>
+  </si>
+  <si>
+    <t>PADOVA ACC</t>
+  </si>
+  <si>
+    <t>Padova ACC</t>
+  </si>
+  <si>
+    <t>LIPPACC</t>
+  </si>
+  <si>
+    <t>PALMA ACC</t>
+  </si>
+  <si>
+    <t>Palma ACC</t>
+  </si>
+  <si>
+    <t>LECPACC</t>
+  </si>
+  <si>
+    <t>PARIS ACC</t>
+  </si>
+  <si>
+    <t>Paris ACC</t>
+  </si>
+  <si>
+    <t>LFFFALL</t>
+  </si>
+  <si>
+    <t>PRAHA ACC</t>
+  </si>
+  <si>
+    <t>Prague ACC</t>
+  </si>
+  <si>
+    <t>LKAAACC</t>
+  </si>
+  <si>
+    <t>REIMS ACC</t>
+  </si>
+  <si>
+    <t>Reims ACC</t>
+  </si>
+  <si>
+    <t>LFEEACC</t>
+  </si>
+  <si>
+    <t>REYKJAVIK ACC</t>
+  </si>
+  <si>
+    <t>Reykjavik ACC</t>
+  </si>
+  <si>
+    <t>BIRDACC</t>
+  </si>
+  <si>
+    <t>RIGA ACC</t>
+  </si>
+  <si>
+    <t>Riga ACC</t>
+  </si>
+  <si>
+    <t>EVRRACC</t>
+  </si>
+  <si>
+    <t>ROMA ACC</t>
+  </si>
+  <si>
+    <t>Rome ACC</t>
+  </si>
+  <si>
+    <t>LIRRACC</t>
+  </si>
+  <si>
+    <t>SANTA MARIA OAC</t>
+  </si>
+  <si>
+    <t>Santa Maria OAC</t>
+  </si>
+  <si>
+    <t>LPPOOAC</t>
+  </si>
+  <si>
+    <t>SARAJEVO ACC</t>
+  </si>
+  <si>
+    <t>Sarajevo ACC</t>
+  </si>
+  <si>
+    <t>LQSBACC</t>
+  </si>
+  <si>
+    <t>SCOTTISH ACC</t>
+  </si>
+  <si>
+    <t>Scottish ACC</t>
+  </si>
+  <si>
+    <t>EGPXALL</t>
+  </si>
+  <si>
+    <t>SEVILLA ACC</t>
+  </si>
+  <si>
+    <t>Seville ACC</t>
+  </si>
+  <si>
+    <t>LECSACC</t>
+  </si>
+  <si>
+    <t>SHANNON ACC</t>
+  </si>
+  <si>
+    <t>Shannon ACC</t>
+  </si>
+  <si>
+    <t>EISNACC</t>
+  </si>
+  <si>
+    <t>SHANWICK OACC</t>
+  </si>
+  <si>
+    <t>Shanwick OACC</t>
+  </si>
+  <si>
+    <t>EGGXOCA</t>
+  </si>
+  <si>
+    <t>SKOPJE ACC</t>
+  </si>
+  <si>
+    <t>Skopje ACC</t>
+  </si>
+  <si>
+    <t>LWSSACC</t>
+  </si>
+  <si>
+    <t>SOFIA ACC</t>
+  </si>
+  <si>
+    <t>Sofia ACC</t>
+  </si>
+  <si>
+    <t>LBSRACC</t>
+  </si>
+  <si>
+    <t>STAVANGER ACC</t>
+  </si>
+  <si>
+    <t>Stavanger ACC</t>
+  </si>
+  <si>
+    <t>ENSVACC</t>
+  </si>
+  <si>
+    <t>STOCKHOLM ACC</t>
+  </si>
+  <si>
+    <t>Stockholm ACC</t>
+  </si>
+  <si>
+    <t>ESOSACC</t>
+  </si>
+  <si>
+    <t>TALLIN ACC</t>
+  </si>
+  <si>
+    <t>Tallin ACC</t>
+  </si>
+  <si>
+    <t>EETTACC</t>
+  </si>
+  <si>
+    <t>TBILISI ACC</t>
+  </si>
+  <si>
+    <t>Tbilisi ACC</t>
+  </si>
+  <si>
+    <t>UGGGACC</t>
+  </si>
+  <si>
+    <t>TEL-AVIV ACC</t>
+  </si>
+  <si>
+    <t>Tel-Aviv ACC</t>
+  </si>
+  <si>
+    <t>LLLLACC</t>
+  </si>
+  <si>
+    <t>TIRANA ACC</t>
+  </si>
+  <si>
+    <t>Tirana ACC</t>
+  </si>
+  <si>
+    <t>LAAAACC</t>
+  </si>
+  <si>
+    <t>VILNIUS ACC</t>
+  </si>
+  <si>
+    <t>Vilnius ACC</t>
+  </si>
+  <si>
+    <t>EYVCACC</t>
+  </si>
+  <si>
+    <t>WARSZAWA ACC</t>
+  </si>
+  <si>
+    <t>Warsaw ACC</t>
+  </si>
+  <si>
+    <t>EPWWACC</t>
+  </si>
+  <si>
+    <t>WIEN ACC</t>
+  </si>
+  <si>
+    <t>Vienna ACC</t>
+  </si>
+  <si>
+    <t>LOVVACC</t>
+  </si>
+  <si>
+    <t>YEREVAN ACC</t>
+  </si>
+  <si>
+    <t>Yerevan ACC</t>
+  </si>
+  <si>
+    <t>UDDDACC</t>
+  </si>
+  <si>
+    <t>ZAGREB ACC</t>
+  </si>
+  <si>
+    <t>Zagreb ACC</t>
+  </si>
+  <si>
+    <t>LDZOACC</t>
+  </si>
+  <si>
+    <t>ZURICH ACC</t>
+  </si>
+  <si>
+    <t>Zurich ACC</t>
+  </si>
+  <si>
+    <t>LSAZACC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -665,8 +1317,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -679,8 +1339,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -701,21 +1367,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.79998168889431442"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.79998168889431442"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -754,7 +1484,7 @@
   <autoFilter ref="F2:H47" xr:uid="{68E28DF6-BC67-4149-BE15-5C30E956B6D0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A3DCCD22-2999-44E1-8245-CC6CF8C82A51}" name="corrected_cz"/>
-    <tableColumn id="3" xr3:uid="{C344E377-A185-4AEA-8EBB-9CD42245E897}" name="cz_proper" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C344E377-A185-4AEA-8EBB-9CD42245E897}" name="cz_proper" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{09539C94-64E6-447B-A935-0128256EE4B8}" name="iso_2letter"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -766,7 +1496,7 @@
   <autoFilter ref="K2:M47" xr:uid="{DC07F4D2-2264-475E-8657-18DD24E4B9B0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C714EEFF-EF4B-404D-BD30-1239DDB1C7CE}" name="daio_zone"/>
-    <tableColumn id="3" xr3:uid="{01CEC5EF-CF6B-430A-A650-FE6D8A2EA212}" name="daio_zone_lc" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{01CEC5EF-CF6B-430A-A650-FE6D8A2EA212}" name="daio_zone_lc" dataDxfId="4">
       <calculatedColumnFormula>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{68CB7EAD-A264-47C3-9969-5842BDB528BB}" name="iso_2letter"/>
@@ -803,7 +1533,23 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{699661C3-76D2-459D-AEC7-8D7B13C306C4}" name="state"/>
     <tableColumn id="2" xr3:uid="{48BDD349-EF16-4557-BE90-D6670E0A4925}" name="iso_2letter"/>
-    <tableColumn id="3" xr3:uid="{A8FDAC0C-0552-4F89-9D61-9BA431327D67}" name="icao_code" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{A8FDAC0C-0552-4F89-9D61-9BA431327D67}" name="icao_code" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3B0B9735-26C8-4572-A44C-72BC473CAB08}" name="Table_ACC_NAMES" displayName="Table_ACC_NAMES" ref="A1:D74" totalsRowShown="0">
+  <autoFilter ref="A1:D74" xr:uid="{3B0B9735-26C8-4572-A44C-72BC473CAB08}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B74">
+    <sortCondition ref="A3:A75"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{D0688728-A473-461B-9D59-1C5B0693D0A3}" name="NM_name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{506F8EA2-492B-4352-A4A3-29BD555CCD5F}" name="Name" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C757E580-579F-457D-829E-B5E46FB51140}" name="iso_2letter"/>
+    <tableColumn id="4" xr3:uid="{2E7D0119-2BEE-4F71-9BE6-0B6C172BB857}" name="ICAO_code" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1108,7 +1854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504966A5-1D6A-4873-89C5-14DFD4258010}">
   <dimension ref="B2:Z47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -3319,6 +4065,1066 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE1B1DA-244C-4D7E-AA08-285D46CCB17C}">
+  <dimension ref="A1:D74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B17" t="s">
+        <v>243</v>
+      </c>
+      <c r="C17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B19" t="s">
+        <v>249</v>
+      </c>
+      <c r="C19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B21" t="s">
+        <v>255</v>
+      </c>
+      <c r="C21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B23" t="s">
+        <v>261</v>
+      </c>
+      <c r="C23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B24" t="s">
+        <v>264</v>
+      </c>
+      <c r="C24" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B25" t="s">
+        <v>267</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B26" t="s">
+        <v>270</v>
+      </c>
+      <c r="C26" t="s">
+        <v>185</v>
+      </c>
+      <c r="D26" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B27" t="s">
+        <v>273</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B28" t="s">
+        <v>276</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B29" t="s">
+        <v>279</v>
+      </c>
+      <c r="C29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D29" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B30" t="s">
+        <v>282</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B31" t="s">
+        <v>285</v>
+      </c>
+      <c r="C31" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B32" t="s">
+        <v>288</v>
+      </c>
+      <c r="C32" t="s">
+        <v>163</v>
+      </c>
+      <c r="D32" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B33" t="s">
+        <v>291</v>
+      </c>
+      <c r="C33" t="s">
+        <v>189</v>
+      </c>
+      <c r="D33" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B34" t="s">
+        <v>294</v>
+      </c>
+      <c r="C34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B35" t="s">
+        <v>297</v>
+      </c>
+      <c r="C35" t="s">
+        <v>195</v>
+      </c>
+      <c r="D35" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B36" t="s">
+        <v>300</v>
+      </c>
+      <c r="C36" t="s">
+        <v>301</v>
+      </c>
+      <c r="D36" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B37" t="s">
+        <v>304</v>
+      </c>
+      <c r="C37" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B38" t="s">
+        <v>307</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B39" t="s">
+        <v>310</v>
+      </c>
+      <c r="C39" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B40" t="s">
+        <v>313</v>
+      </c>
+      <c r="C40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B41" t="s">
+        <v>316</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B42" t="s">
+        <v>319</v>
+      </c>
+      <c r="C42" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B43" t="s">
+        <v>322</v>
+      </c>
+      <c r="C43" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B44" t="s">
+        <v>325</v>
+      </c>
+      <c r="C44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B45" t="s">
+        <v>328</v>
+      </c>
+      <c r="C45" t="s">
+        <v>195</v>
+      </c>
+      <c r="D45" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B46" t="s">
+        <v>331</v>
+      </c>
+      <c r="C46" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B47" t="s">
+        <v>334</v>
+      </c>
+      <c r="C47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B48" t="s">
+        <v>337</v>
+      </c>
+      <c r="C48" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B49" t="s">
+        <v>340</v>
+      </c>
+      <c r="C49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B50" t="s">
+        <v>343</v>
+      </c>
+      <c r="C50" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="B51" t="s">
+        <v>346</v>
+      </c>
+      <c r="C51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B52" t="s">
+        <v>349</v>
+      </c>
+      <c r="C52" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B53" t="s">
+        <v>352</v>
+      </c>
+      <c r="C53" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B54" t="s">
+        <v>355</v>
+      </c>
+      <c r="C54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B55" t="s">
+        <v>358</v>
+      </c>
+      <c r="C55" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B56" t="s">
+        <v>361</v>
+      </c>
+      <c r="C56" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B57" t="s">
+        <v>364</v>
+      </c>
+      <c r="C57" t="s">
+        <v>189</v>
+      </c>
+      <c r="D57" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B58" t="s">
+        <v>367</v>
+      </c>
+      <c r="C58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B59" t="s">
+        <v>370</v>
+      </c>
+      <c r="C59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D59" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B60" t="s">
+        <v>373</v>
+      </c>
+      <c r="C60" t="s">
+        <v>189</v>
+      </c>
+      <c r="D60" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B61" t="s">
+        <v>376</v>
+      </c>
+      <c r="C61" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B62" t="s">
+        <v>379</v>
+      </c>
+      <c r="C62" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B63" t="s">
+        <v>382</v>
+      </c>
+      <c r="C63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D63" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="B64" t="s">
+        <v>385</v>
+      </c>
+      <c r="C64" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="B65" t="s">
+        <v>388</v>
+      </c>
+      <c r="C65" t="s">
+        <v>55</v>
+      </c>
+      <c r="D65" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="B66" t="s">
+        <v>391</v>
+      </c>
+      <c r="C66" t="s">
+        <v>67</v>
+      </c>
+      <c r="D66" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B67" t="s">
+        <v>394</v>
+      </c>
+      <c r="C67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="B68" t="s">
+        <v>397</v>
+      </c>
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B69" t="s">
+        <v>400</v>
+      </c>
+      <c r="C69" t="s">
+        <v>104</v>
+      </c>
+      <c r="D69" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B70" t="s">
+        <v>403</v>
+      </c>
+      <c r="C70" t="s">
+        <v>141</v>
+      </c>
+      <c r="D70" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B71" t="s">
+        <v>406</v>
+      </c>
+      <c r="C71" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B72" t="s">
+        <v>409</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B73" t="s">
+        <v>412</v>
+      </c>
+      <c r="C73" t="s">
+        <v>36</v>
+      </c>
+      <c r="D73" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="B74" t="s">
+        <v>415</v>
+      </c>
+      <c r="C74" t="s">
+        <v>180</v>
+      </c>
+      <c r="D74" t="s">
+        <v>416</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{fd60f3b8-f236-4830-aecc-da0a7fc54679}" enabled="1" method="Standard" siteId="{76f33c20-5979-4408-adf7-8b3c4be95e52}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
corrected ap st des base table
</commit_message>
<xml_diff>
--- a/stakeholder_lists.xlsx
+++ b/stakeholder_lists.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\mobile-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D921B456-CA09-4899-88FF-41DCD2DDF33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1873EF8C-2E88-420F-B619-3D58F0E73F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="1" xr2:uid="{17D0CF8C-6239-4396-93EE-ED3916C7EA4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="2" xr2:uid="{17D0CF8C-6239-4396-93EE-ED3916C7EA4B}"/>
   </bookViews>
   <sheets>
     <sheet name="state_lists" sheetId="1" r:id="rId1"/>
     <sheet name="acc_lists" sheetId="2" r:id="rId2"/>
+    <sheet name="ansp_lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="501">
   <si>
     <t>state</t>
   </si>
@@ -1288,6 +1289,258 @@
   </si>
   <si>
     <t>LSAZACC</t>
+  </si>
+  <si>
+    <t>ANSP_CODE</t>
+  </si>
+  <si>
+    <t>ANSP_NAME</t>
+  </si>
+  <si>
+    <t>PRU_ID</t>
+  </si>
+  <si>
+    <t>IE_ANSP</t>
+  </si>
+  <si>
+    <t>AirNav Ireland</t>
+  </si>
+  <si>
+    <t>AL_ANSP</t>
+  </si>
+  <si>
+    <t>Albcontrol</t>
+  </si>
+  <si>
+    <t>CZ_ANSP</t>
+  </si>
+  <si>
+    <t>ANS CR</t>
+  </si>
+  <si>
+    <t>AM_ANSP</t>
+  </si>
+  <si>
+    <t>ARMATS</t>
+  </si>
+  <si>
+    <t>AT_ANSP</t>
+  </si>
+  <si>
+    <t>Austro Control</t>
+  </si>
+  <si>
+    <t>NO_ANSP</t>
+  </si>
+  <si>
+    <t>Avinor</t>
+  </si>
+  <si>
+    <t>BA_ANSP</t>
+  </si>
+  <si>
+    <t>BHANSA</t>
+  </si>
+  <si>
+    <t>BG_ANSP</t>
+  </si>
+  <si>
+    <t>BULATSA</t>
+  </si>
+  <si>
+    <t>HR_ANSP</t>
+  </si>
+  <si>
+    <t>Croatia Control</t>
+  </si>
+  <si>
+    <t>CY_ANSP</t>
+  </si>
+  <si>
+    <t>DCAC Cyprus</t>
+  </si>
+  <si>
+    <t>DE_ANSP</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>TR_ANSP</t>
+  </si>
+  <si>
+    <t>DHMI</t>
+  </si>
+  <si>
+    <t>FR_ANSP</t>
+  </si>
+  <si>
+    <t>DSNA</t>
+  </si>
+  <si>
+    <t>EE_ANSP</t>
+  </si>
+  <si>
+    <t>EANS</t>
+  </si>
+  <si>
+    <t>ES_ANSP</t>
+  </si>
+  <si>
+    <t>ENAIRE</t>
+  </si>
+  <si>
+    <t>IT_ANSP</t>
+  </si>
+  <si>
+    <t>ENAV</t>
+  </si>
+  <si>
+    <t>FI_ANSP</t>
+  </si>
+  <si>
+    <t>Fintraffic ANS</t>
+  </si>
+  <si>
+    <t>GR_ANSP</t>
+  </si>
+  <si>
+    <t>HASP</t>
+  </si>
+  <si>
+    <t>HU_ANSP</t>
+  </si>
+  <si>
+    <t>HungaroControl (EC)</t>
+  </si>
+  <si>
+    <t>IS_ANSP</t>
+  </si>
+  <si>
+    <t>Isavia</t>
+  </si>
+  <si>
+    <t>IL_ANSP</t>
+  </si>
+  <si>
+    <t>Israel AA</t>
+  </si>
+  <si>
+    <t>SE_ANSP</t>
+  </si>
+  <si>
+    <t>LFV</t>
+  </si>
+  <si>
+    <t>LV_ANSP</t>
+  </si>
+  <si>
+    <t>LGS</t>
+  </si>
+  <si>
+    <t>SK_ANSP</t>
+  </si>
+  <si>
+    <t>LPS</t>
+  </si>
+  <si>
+    <t>NL_ANSP</t>
+  </si>
+  <si>
+    <t>LVNL</t>
+  </si>
+  <si>
+    <t>MT_ANSP</t>
+  </si>
+  <si>
+    <t>MATS</t>
+  </si>
+  <si>
+    <t>MK_ANSP</t>
+  </si>
+  <si>
+    <t>M-NAV</t>
+  </si>
+  <si>
+    <t>MD_ANSP</t>
+  </si>
+  <si>
+    <t>MOLDATSA</t>
+  </si>
+  <si>
+    <t>MAS_ANSP</t>
+  </si>
+  <si>
+    <t>GB_ANSP</t>
+  </si>
+  <si>
+    <t>NATS (Continental)</t>
+  </si>
+  <si>
+    <t>PT_ANSP</t>
+  </si>
+  <si>
+    <t>NAV Portugal (Continental)</t>
+  </si>
+  <si>
+    <t>DK_ANSP</t>
+  </si>
+  <si>
+    <t>NAVIAIR</t>
+  </si>
+  <si>
+    <t>MA_ANSP</t>
+  </si>
+  <si>
+    <t>ONDA</t>
+  </si>
+  <si>
+    <t>LT_ANSP</t>
+  </si>
+  <si>
+    <t>Oro Navigacija</t>
+  </si>
+  <si>
+    <t>PL_ANSP</t>
+  </si>
+  <si>
+    <t>PANSA</t>
+  </si>
+  <si>
+    <t>RO_ANSP</t>
+  </si>
+  <si>
+    <t>ROMATSA</t>
+  </si>
+  <si>
+    <t>GE_ANSP</t>
+  </si>
+  <si>
+    <t>Sakaeronavigatsia</t>
+  </si>
+  <si>
+    <t>BE_ANSP</t>
+  </si>
+  <si>
+    <t>skeyes</t>
+  </si>
+  <si>
+    <t>CH_ANSP</t>
+  </si>
+  <si>
+    <t>Skyguide</t>
+  </si>
+  <si>
+    <t>SI_ANSP</t>
+  </si>
+  <si>
+    <t>Slovenia Control</t>
+  </si>
+  <si>
+    <t>MERS_ANSP</t>
+  </si>
+  <si>
+    <t>SMATSA</t>
   </si>
 </sst>
 </file>
@@ -1403,7 +1656,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1484,7 +1740,7 @@
   <autoFilter ref="F2:H47" xr:uid="{68E28DF6-BC67-4149-BE15-5C30E956B6D0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A3DCCD22-2999-44E1-8245-CC6CF8C82A51}" name="corrected_cz"/>
-    <tableColumn id="3" xr3:uid="{C344E377-A185-4AEA-8EBB-9CD42245E897}" name="cz_proper" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{C344E377-A185-4AEA-8EBB-9CD42245E897}" name="cz_proper" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{09539C94-64E6-447B-A935-0128256EE4B8}" name="iso_2letter"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1496,7 +1752,7 @@
   <autoFilter ref="K2:M47" xr:uid="{DC07F4D2-2264-475E-8657-18DD24E4B9B0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C714EEFF-EF4B-404D-BD30-1239DDB1C7CE}" name="daio_zone"/>
-    <tableColumn id="3" xr3:uid="{01CEC5EF-CF6B-430A-A650-FE6D8A2EA212}" name="daio_zone_lc" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{01CEC5EF-CF6B-430A-A650-FE6D8A2EA212}" name="daio_zone_lc" dataDxfId="5">
       <calculatedColumnFormula>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{68CB7EAD-A264-47C3-9969-5842BDB528BB}" name="iso_2letter"/>
@@ -1533,7 +1789,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{699661C3-76D2-459D-AEC7-8D7B13C306C4}" name="state"/>
     <tableColumn id="2" xr3:uid="{48BDD349-EF16-4557-BE90-D6670E0A4925}" name="iso_2letter"/>
-    <tableColumn id="3" xr3:uid="{A8FDAC0C-0552-4F89-9D61-9BA431327D67}" name="icao_code" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A8FDAC0C-0552-4F89-9D61-9BA431327D67}" name="icao_code" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1546,10 +1802,22 @@
     <sortCondition ref="A3:A75"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D0688728-A473-461B-9D59-1C5B0693D0A3}" name="NM_name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{506F8EA2-492B-4352-A4A3-29BD555CCD5F}" name="Name" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{D0688728-A473-461B-9D59-1C5B0693D0A3}" name="NM_name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{506F8EA2-492B-4352-A4A3-29BD555CCD5F}" name="Name" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{C757E580-579F-457D-829E-B5E46FB51140}" name="iso_2letter"/>
-    <tableColumn id="4" xr3:uid="{2E7D0119-2BEE-4F71-9BE6-0B6C172BB857}" name="ICAO_code" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{2E7D0119-2BEE-4F71-9BE6-0B6C172BB857}" name="ICAO_code" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FA35717E-13AB-4160-B118-09C179253D55}" name="Table_ANSP_NAMES" displayName="Table_ANSP_NAMES" ref="A1:C42" totalsRowShown="0">
+  <autoFilter ref="A1:C42" xr:uid="{FA35717E-13AB-4160-B118-09C179253D55}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{5913F9FF-BF18-4F38-BAF9-BF6580705921}" name="ANSP_CODE"/>
+    <tableColumn id="2" xr3:uid="{BE60DAF5-A5C4-4231-A544-FF07431919B8}" name="ANSP_NAME"/>
+    <tableColumn id="3" xr3:uid="{ACA69020-37C6-45DE-A1BE-40ED68D12C26}" name="PRU_ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4069,7 +4337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE1B1DA-244C-4D7E-AA08-285D46CCB17C}">
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -5125,6 +5393,491 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED1E104-9062-4EAF-9E42-F22F5508C47F}">
+  <dimension ref="A1:C42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B5" t="s">
+        <v>427</v>
+      </c>
+      <c r="C5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>428</v>
+      </c>
+      <c r="B6" t="s">
+        <v>429</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>430</v>
+      </c>
+      <c r="B7" t="s">
+        <v>431</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B8" t="s">
+        <v>433</v>
+      </c>
+      <c r="C8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>434</v>
+      </c>
+      <c r="B9" t="s">
+        <v>435</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>436</v>
+      </c>
+      <c r="B10" t="s">
+        <v>437</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>438</v>
+      </c>
+      <c r="B11" t="s">
+        <v>439</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>440</v>
+      </c>
+      <c r="B12" t="s">
+        <v>441</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>442</v>
+      </c>
+      <c r="B13" t="s">
+        <v>443</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>444</v>
+      </c>
+      <c r="B14" t="s">
+        <v>445</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>446</v>
+      </c>
+      <c r="B15" t="s">
+        <v>447</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>448</v>
+      </c>
+      <c r="B16" t="s">
+        <v>449</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>450</v>
+      </c>
+      <c r="B17" t="s">
+        <v>451</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>452</v>
+      </c>
+      <c r="B18" t="s">
+        <v>453</v>
+      </c>
+      <c r="C18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>454</v>
+      </c>
+      <c r="B19" t="s">
+        <v>455</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>456</v>
+      </c>
+      <c r="B20" t="s">
+        <v>457</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>458</v>
+      </c>
+      <c r="B21" t="s">
+        <v>459</v>
+      </c>
+      <c r="C21">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>460</v>
+      </c>
+      <c r="B22" t="s">
+        <v>461</v>
+      </c>
+      <c r="C22">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>462</v>
+      </c>
+      <c r="B23" t="s">
+        <v>463</v>
+      </c>
+      <c r="C23">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>464</v>
+      </c>
+      <c r="B24" t="s">
+        <v>465</v>
+      </c>
+      <c r="C24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>466</v>
+      </c>
+      <c r="B25" t="s">
+        <v>467</v>
+      </c>
+      <c r="C25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>468</v>
+      </c>
+      <c r="B26" t="s">
+        <v>469</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>470</v>
+      </c>
+      <c r="B27" t="s">
+        <v>471</v>
+      </c>
+      <c r="C27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>472</v>
+      </c>
+      <c r="B28" t="s">
+        <v>473</v>
+      </c>
+      <c r="C28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>474</v>
+      </c>
+      <c r="B29" t="s">
+        <v>475</v>
+      </c>
+      <c r="C29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>476</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>477</v>
+      </c>
+      <c r="B31" t="s">
+        <v>478</v>
+      </c>
+      <c r="C31">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>479</v>
+      </c>
+      <c r="B32" t="s">
+        <v>480</v>
+      </c>
+      <c r="C32">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>481</v>
+      </c>
+      <c r="B33" t="s">
+        <v>482</v>
+      </c>
+      <c r="C33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>483</v>
+      </c>
+      <c r="B34" t="s">
+        <v>484</v>
+      </c>
+      <c r="C34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>485</v>
+      </c>
+      <c r="B35" t="s">
+        <v>486</v>
+      </c>
+      <c r="C35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>487</v>
+      </c>
+      <c r="B36" t="s">
+        <v>488</v>
+      </c>
+      <c r="C36">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>489</v>
+      </c>
+      <c r="B37" t="s">
+        <v>490</v>
+      </c>
+      <c r="C37">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>491</v>
+      </c>
+      <c r="B38" t="s">
+        <v>492</v>
+      </c>
+      <c r="C38">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>493</v>
+      </c>
+      <c r="B39" t="s">
+        <v>494</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>495</v>
+      </c>
+      <c r="B40" t="s">
+        <v>496</v>
+      </c>
+      <c r="C40">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>497</v>
+      </c>
+      <c r="B41" t="s">
+        <v>498</v>
+      </c>
+      <c r="C41">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>499</v>
+      </c>
+      <c r="B42" t="s">
+        <v>500</v>
+      </c>
+      <c r="C42">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{fd60f3b8-f236-4830-aecc-da0a7fc54679}" enabled="1" method="Standard" siteId="{76f33c20-5979-4408-adf7-8b3c4be95e52}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
removed maastricht from state list
</commit_message>
<xml_diff>
--- a/stakeholder_lists.xlsx
+++ b/stakeholder_lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\mobile-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79282675-2EDE-478B-8F87-F96488380E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343AF638-C776-4EE9-9D0A-E9258E5822B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="2" xr2:uid="{17D0CF8C-6239-4396-93EE-ED3916C7EA4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{17D0CF8C-6239-4396-93EE-ED3916C7EA4B}"/>
   </bookViews>
   <sheets>
     <sheet name="state_lists" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="500">
   <si>
     <t>state</t>
   </si>
@@ -371,9 +371,6 @@
   </si>
   <si>
     <t>EL</t>
-  </si>
-  <si>
-    <t>Maastricht</t>
   </si>
   <si>
     <t>MUAC</t>
@@ -1725,8 +1722,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FD9F205-62A8-466E-8EE7-E7D537C52746}" name="Table_STATE_ISO" displayName="Table_STATE_ISO" ref="B2:C47" totalsRowShown="0">
-  <autoFilter ref="B2:C47" xr:uid="{B65F2BB6-6CE7-4EE3-B2BB-2DE4E20413D4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FD9F205-62A8-466E-8EE7-E7D537C52746}" name="Table_STATE_ISO" displayName="Table_STATE_ISO" ref="B2:C46" totalsRowShown="0">
+  <autoFilter ref="B2:C46" xr:uid="{B65F2BB6-6CE7-4EE3-B2BB-2DE4E20413D4}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{692F2180-21D0-43B0-A43B-F1E15E55CC29}" name="state"/>
     <tableColumn id="2" xr3:uid="{4378186E-C9C6-44DD-BC6A-78736082D237}" name="iso_2letter"/>
@@ -1748,8 +1745,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C4BE6A1-8EAC-4C50-96C2-6F03C88D8E92}" name="Table_DAIO_ISO" displayName="Table_DAIO_ISO" ref="K2:M47" totalsRowShown="0">
-  <autoFilter ref="K2:M47" xr:uid="{DC07F4D2-2264-475E-8657-18DD24E4B9B0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C4BE6A1-8EAC-4C50-96C2-6F03C88D8E92}" name="Table_DAIO_ISO" displayName="Table_DAIO_ISO" ref="K2:M46" totalsRowShown="0">
+  <autoFilter ref="K2:M46" xr:uid="{DC07F4D2-2264-475E-8657-18DD24E4B9B0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C714EEFF-EF4B-404D-BD30-1239DDB1C7CE}" name="daio_zone"/>
     <tableColumn id="3" xr3:uid="{01CEC5EF-CF6B-430A-A650-FE6D8A2EA212}" name="daio_zone_lc" dataDxfId="5">
@@ -1784,8 +1781,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{07D022ED-2FDA-4248-95C6-BE6CA4318242}" name="Table_STATE_ISO20" displayName="Table_STATE_ISO20" ref="X2:Z47" totalsRowShown="0">
-  <autoFilter ref="X2:Z47" xr:uid="{FD3F3339-CE62-4BFD-9263-3BAAED552141}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{07D022ED-2FDA-4248-95C6-BE6CA4318242}" name="Table_STATE_ISO20" displayName="Table_STATE_ISO20" ref="X2:Z46" totalsRowShown="0">
+  <autoFilter ref="X2:Z46" xr:uid="{FD3F3339-CE62-4BFD-9263-3BAAED552141}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{699661C3-76D2-459D-AEC7-8D7B13C306C4}" name="state"/>
     <tableColumn id="2" xr3:uid="{48BDD349-EF16-4557-BE90-D6670E0A4925}" name="iso_2letter"/>
@@ -2122,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504966A5-1D6A-4873-89C5-14DFD4258010}">
   <dimension ref="B2:Z47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27:Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3343,10 +3340,10 @@
     </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F27" t="s">
         <v>84</v>
@@ -3355,190 +3352,190 @@
         <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K27" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="L27" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>maastricht</v>
+        <v>malta</v>
       </c>
       <c r="M27" t="s">
+        <v>113</v>
+      </c>
+      <c r="P27" t="s">
         <v>112</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>113</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="T27" t="s">
         <v>114</v>
       </c>
-      <c r="T27" t="s">
-        <v>115</v>
-      </c>
       <c r="U27" t="s">
+        <v>113</v>
+      </c>
+      <c r="X27" t="s">
         <v>114</v>
       </c>
-      <c r="X27" t="s">
-        <v>111</v>
-      </c>
       <c r="Y27" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Z27" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C28" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G28" t="s">
         <v>114</v>
       </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
         <v>113</v>
       </c>
-      <c r="G28" t="s">
-        <v>115</v>
-      </c>
-      <c r="H28" t="s">
-        <v>114</v>
-      </c>
       <c r="K28" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L28" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>malta</v>
+        <v>moldova</v>
       </c>
       <c r="M28" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="P28" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q28" t="s">
         <v>116</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="T28" t="s">
         <v>117</v>
       </c>
-      <c r="T28" t="s">
-        <v>118</v>
-      </c>
       <c r="U28" t="s">
+        <v>116</v>
+      </c>
+      <c r="X28" t="s">
         <v>117</v>
       </c>
-      <c r="X28" t="s">
-        <v>115</v>
-      </c>
       <c r="Y28" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="Z28" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C29" t="s">
+        <v>121</v>
+      </c>
+      <c r="F29" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" t="s">
         <v>117</v>
       </c>
-      <c r="F29" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" t="s">
-        <v>118</v>
-      </c>
       <c r="H29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K29" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="L29" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>moldova</v>
+        <v>serbia/montenegro</v>
       </c>
       <c r="M29" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="P29" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q29" t="s">
         <v>121</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="T29" t="s">
         <v>122</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
         <v>123</v>
       </c>
-      <c r="U29" t="s">
+      <c r="X29" t="s">
         <v>124</v>
       </c>
-      <c r="X29" t="s">
-        <v>118</v>
-      </c>
       <c r="Y29" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="Z29" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" t="s">
         <v>125</v>
       </c>
-      <c r="C30" t="s">
+      <c r="G30" t="s">
+        <v>126</v>
+      </c>
+      <c r="H30" t="s">
+        <v>121</v>
+      </c>
+      <c r="K30" t="s">
         <v>122</v>
-      </c>
-      <c r="F30" t="s">
-        <v>126</v>
-      </c>
-      <c r="G30" t="s">
-        <v>127</v>
-      </c>
-      <c r="H30" t="s">
-        <v>122</v>
-      </c>
-      <c r="K30" t="s">
-        <v>128</v>
       </c>
       <c r="L30" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>serbia/montenegro</v>
+        <v>morocco</v>
       </c>
       <c r="M30" t="s">
+        <v>123</v>
+      </c>
+      <c r="P30" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>129</v>
+      </c>
+      <c r="T30" t="s">
+        <v>127</v>
+      </c>
+      <c r="U30" t="s">
+        <v>121</v>
+      </c>
+      <c r="X30" t="s">
         <v>122</v>
       </c>
-      <c r="P30" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>130</v>
-      </c>
-      <c r="T30" t="s">
-        <v>128</v>
-      </c>
-      <c r="U30" t="s">
-        <v>122</v>
-      </c>
-      <c r="X30" t="s">
-        <v>125</v>
-      </c>
       <c r="Y30" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Z30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F31" t="s">
         <v>84</v>
@@ -3547,614 +3544,614 @@
         <v>85</v>
       </c>
       <c r="H31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K31" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="L31" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>morocco</v>
+        <v>netherlands</v>
       </c>
       <c r="M31" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="P31" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q31" t="s">
         <v>132</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="T31" t="s">
         <v>133</v>
       </c>
-      <c r="T31" t="s">
-        <v>134</v>
-      </c>
       <c r="U31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X31" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="Y31" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="Z31" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F32" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" t="s">
+        <v>133</v>
+      </c>
+      <c r="H32" t="s">
         <v>129</v>
       </c>
-      <c r="G32" t="s">
-        <v>134</v>
-      </c>
-      <c r="H32" t="s">
-        <v>130</v>
-      </c>
       <c r="K32" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="L32" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>netherlands</v>
+        <v>north macedonia</v>
       </c>
       <c r="M32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="P32" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q32" t="s">
         <v>136</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="T32" t="s">
         <v>137</v>
       </c>
-      <c r="T32" t="s">
-        <v>138</v>
-      </c>
       <c r="U32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X32" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="Y32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="Z32" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F33" t="s">
+        <v>131</v>
+      </c>
+      <c r="G33" t="s">
+        <v>137</v>
+      </c>
+      <c r="H33" t="s">
         <v>132</v>
       </c>
-      <c r="G33" t="s">
-        <v>138</v>
-      </c>
-      <c r="H33" t="s">
-        <v>133</v>
-      </c>
       <c r="K33" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="L33" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>north macedonia</v>
+        <v>norway</v>
       </c>
       <c r="M33" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="P33" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q33" t="s">
         <v>140</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="T33" t="s">
         <v>141</v>
       </c>
-      <c r="T33" t="s">
-        <v>142</v>
-      </c>
       <c r="U33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="X33" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="Y33" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="Z33" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" t="s">
+        <v>140</v>
+      </c>
+      <c r="F34" t="s">
         <v>144</v>
       </c>
-      <c r="C34" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" t="s">
-        <v>145</v>
-      </c>
       <c r="G34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K34" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="L34" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>norway</v>
+        <v>poland</v>
       </c>
       <c r="M34" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="P34" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q34" t="s">
         <v>146</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="T34" t="s">
         <v>147</v>
       </c>
-      <c r="T34" t="s">
-        <v>148</v>
-      </c>
       <c r="U34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X34" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="Y34" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="Z34" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F35" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" t="s">
+        <v>147</v>
+      </c>
+      <c r="H35" t="s">
         <v>140</v>
       </c>
-      <c r="G35" t="s">
-        <v>148</v>
-      </c>
-      <c r="H35" t="s">
-        <v>141</v>
-      </c>
       <c r="K35" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="L35" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>poland</v>
+        <v>portugal</v>
       </c>
       <c r="M35" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="P35" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q35" t="s">
         <v>150</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="T35" t="s">
         <v>151</v>
       </c>
-      <c r="T35" t="s">
-        <v>152</v>
-      </c>
       <c r="U35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="X35" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="Y35" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="Z35" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C36" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K36" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="L36" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>portugal</v>
+        <v>romania</v>
       </c>
       <c r="M36" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="P36" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q36" t="s">
         <v>154</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="T36" t="s">
         <v>155</v>
       </c>
-      <c r="T36" t="s">
-        <v>156</v>
-      </c>
       <c r="U36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X36" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="Y36" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="Z36" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C37" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F37" t="s">
+        <v>149</v>
+      </c>
+      <c r="G37" t="s">
+        <v>155</v>
+      </c>
+      <c r="H37" t="s">
         <v>150</v>
       </c>
-      <c r="G37" t="s">
-        <v>156</v>
-      </c>
-      <c r="H37" t="s">
-        <v>151</v>
-      </c>
       <c r="K37" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="L37" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>romania</v>
+        <v>serbia/montenegro</v>
       </c>
       <c r="M37" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="P37" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q37" t="s">
         <v>158</v>
       </c>
-      <c r="Q37" t="s">
-        <v>159</v>
-      </c>
       <c r="T37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X37" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="Y37" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="Z37" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F38" t="s">
+        <v>125</v>
+      </c>
+      <c r="G38" t="s">
         <v>126</v>
       </c>
-      <c r="G38" t="s">
-        <v>127</v>
-      </c>
       <c r="H38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K38" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="L38" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>serbia/montenegro</v>
+        <v>slovakia</v>
       </c>
       <c r="M38" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="P38" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q38" t="s">
         <v>162</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="T38" t="s">
         <v>163</v>
       </c>
-      <c r="T38" t="s">
-        <v>164</v>
-      </c>
       <c r="U38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="X38" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="Y38" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="Z38" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" t="s">
+        <v>162</v>
+      </c>
+      <c r="F39" t="s">
         <v>164</v>
       </c>
-      <c r="C39" t="s">
-        <v>159</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>165</v>
       </c>
-      <c r="G39" t="s">
-        <v>166</v>
-      </c>
       <c r="H39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K39" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="L39" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>slovakia</v>
+        <v>slovenia</v>
       </c>
       <c r="M39" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="P39" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q39" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="Q39" s="4" t="s">
+      <c r="T39" t="s">
         <v>168</v>
       </c>
-      <c r="T39" t="s">
-        <v>169</v>
-      </c>
       <c r="U39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X39" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="Y39" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="Z39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" t="s">
+        <v>161</v>
+      </c>
+      <c r="G40" t="s">
+        <v>168</v>
+      </c>
+      <c r="H40" t="s">
+        <v>162</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="L40" s="4" t="str">
+        <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
+        <v>spain continental</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="P40" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="40" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>169</v>
-      </c>
-      <c r="C40" t="s">
-        <v>163</v>
-      </c>
-      <c r="F40" t="s">
-        <v>162</v>
-      </c>
-      <c r="G40" t="s">
-        <v>169</v>
-      </c>
-      <c r="H40" t="s">
-        <v>163</v>
-      </c>
-      <c r="K40" t="s">
-        <v>169</v>
-      </c>
-      <c r="L40" t="str">
-        <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>slovenia</v>
-      </c>
-      <c r="M40" t="s">
-        <v>163</v>
-      </c>
-      <c r="P40" t="s">
+      <c r="Q40" t="s">
         <v>171</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="T40" s="4" t="s">
         <v>172</v>
-      </c>
-      <c r="T40" s="4" t="s">
-        <v>173</v>
       </c>
       <c r="U40" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="X40" t="s">
-        <v>169</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>163</v>
+      <c r="X40" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y40" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="Z40" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F41" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="H41" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="L41" s="4" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>spain continental</v>
+        <v>spain canaries</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>168</v>
+        <v>39</v>
       </c>
       <c r="P41" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q41" t="s">
         <v>179</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="T41" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="T41" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="U41" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X41" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="Y41" s="4" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="Z41" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>185</v>
+      </c>
+      <c r="C42" t="s">
+        <v>171</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="G42" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K42" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="L42" s="4" t="str">
+      <c r="K42" t="s">
+        <v>185</v>
+      </c>
+      <c r="L42" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>spain canaries</v>
-      </c>
-      <c r="M42" s="4" t="s">
-        <v>39</v>
+        <v>sweden</v>
+      </c>
+      <c r="M42" t="s">
+        <v>171</v>
       </c>
       <c r="P42" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q42" t="s">
         <v>184</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="T42" t="s">
         <v>185</v>
       </c>
-      <c r="T42" t="s">
-        <v>186</v>
-      </c>
       <c r="U42" t="s">
-        <v>172</v>
-      </c>
-      <c r="X42" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y42" s="4" t="s">
-        <v>168</v>
+        <v>171</v>
+      </c>
+      <c r="X42" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>171</v>
       </c>
       <c r="Z42" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C43" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="F43" t="s">
+        <v>170</v>
+      </c>
+      <c r="G43" t="s">
+        <v>185</v>
+      </c>
+      <c r="H43" t="s">
         <v>171</v>
       </c>
-      <c r="G43" t="s">
-        <v>186</v>
-      </c>
-      <c r="H43" t="s">
-        <v>172</v>
-      </c>
       <c r="K43" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="L43" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>sweden</v>
+        <v>switzerland</v>
       </c>
       <c r="M43" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="P43" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q43" t="s">
         <v>188</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="T43" t="s">
         <v>189</v>
       </c>
-      <c r="T43" t="s">
-        <v>190</v>
-      </c>
       <c r="U43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="X43" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="Y43" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="Z43" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="2:26" x14ac:dyDescent="0.25">
@@ -4162,161 +4159,136 @@
         <v>190</v>
       </c>
       <c r="C44" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F44" t="s">
+        <v>178</v>
+      </c>
+      <c r="G44" t="s">
+        <v>189</v>
+      </c>
+      <c r="H44" t="s">
         <v>179</v>
-      </c>
-      <c r="G44" t="s">
-        <v>190</v>
-      </c>
-      <c r="H44" t="s">
-        <v>180</v>
       </c>
       <c r="K44" t="s">
         <v>190</v>
       </c>
       <c r="L44" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>switzerland</v>
+        <v>türkiye</v>
       </c>
       <c r="M44" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="T44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U44" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="X44" t="s">
         <v>190</v>
       </c>
       <c r="Y44" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="Z44" t="s">
-        <v>192</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C45" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="F45" t="s">
+        <v>183</v>
+      </c>
+      <c r="G45" t="s">
+        <v>190</v>
+      </c>
+      <c r="H45" t="s">
         <v>184</v>
       </c>
-      <c r="G45" t="s">
-        <v>191</v>
-      </c>
-      <c r="H45" t="s">
-        <v>185</v>
-      </c>
       <c r="K45" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="L45" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>türkiye</v>
+        <v>ukraine</v>
       </c>
       <c r="M45" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="T45" t="s">
+        <v>192</v>
+      </c>
+      <c r="U45" t="s">
+        <v>188</v>
+      </c>
+      <c r="X45" t="s">
         <v>193</v>
       </c>
-      <c r="U45" t="s">
-        <v>189</v>
-      </c>
-      <c r="X45" t="s">
-        <v>191</v>
-      </c>
       <c r="Y45" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="Z45" t="s">
-        <v>104</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>196</v>
+      </c>
+      <c r="C46" t="s">
+        <v>188</v>
+      </c>
+      <c r="F46" t="s">
+        <v>193</v>
+      </c>
+      <c r="G46" t="s">
+        <v>193</v>
+      </c>
+      <c r="H46" t="s">
         <v>194</v>
       </c>
-      <c r="C46" t="s">
-        <v>195</v>
-      </c>
-      <c r="F46" t="s">
-        <v>194</v>
-      </c>
-      <c r="G46" t="s">
-        <v>194</v>
-      </c>
-      <c r="H46" t="s">
-        <v>195</v>
-      </c>
       <c r="K46" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="L46" t="str">
         <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>ukraine</v>
+        <v>united kingdom</v>
       </c>
       <c r="M46" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="T46" t="s">
+        <v>193</v>
+      </c>
+      <c r="U46" t="s">
         <v>194</v>
       </c>
-      <c r="U46" t="s">
-        <v>195</v>
-      </c>
       <c r="X46" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="Y46" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Z46" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>197</v>
+      </c>
+      <c r="G47" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="47" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>197</v>
-      </c>
-      <c r="C47" t="s">
-        <v>189</v>
-      </c>
-      <c r="F47" t="s">
-        <v>198</v>
-      </c>
-      <c r="G47" t="s">
-        <v>197</v>
-      </c>
       <c r="H47" t="s">
-        <v>189</v>
-      </c>
-      <c r="K47" t="s">
-        <v>197</v>
-      </c>
-      <c r="L47" t="str">
-        <f>LOWER(Table_DAIO_ISO[[#This Row],[daio_zone]])</f>
-        <v>united kingdom</v>
-      </c>
-      <c r="M47" t="s">
-        <v>189</v>
-      </c>
-      <c r="X47" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z47" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -4351,1038 +4323,1038 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" t="s">
         <v>200</v>
-      </c>
-      <c r="B1" t="s">
-        <v>201</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" t="s">
         <v>203</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
         <v>204</v>
-      </c>
-      <c r="C2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s">
         <v>206</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
         <v>207</v>
-      </c>
-      <c r="C3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" t="s">
         <v>209</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" t="s">
         <v>210</v>
-      </c>
-      <c r="C4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" t="s">
         <v>212</v>
-      </c>
-      <c r="B5" t="s">
-        <v>213</v>
       </c>
       <c r="C5" t="s">
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" t="s">
         <v>215</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" t="s">
         <v>216</v>
-      </c>
-      <c r="C6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D6" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" t="s">
         <v>218</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
         <v>219</v>
-      </c>
-      <c r="C7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" t="s">
         <v>218</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" t="s">
         <v>219</v>
-      </c>
-      <c r="C8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" t="s">
         <v>221</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" t="s">
         <v>222</v>
-      </c>
-      <c r="C9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" t="s">
         <v>224</v>
-      </c>
-      <c r="B10" t="s">
-        <v>225</v>
       </c>
       <c r="C10" t="s">
         <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" t="s">
         <v>227</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" t="s">
         <v>228</v>
-      </c>
-      <c r="C11" t="s">
-        <v>159</v>
-      </c>
-      <c r="D11" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12" t="s">
         <v>230</v>
-      </c>
-      <c r="B12" t="s">
-        <v>231</v>
       </c>
       <c r="C12" t="s">
         <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" t="s">
         <v>233</v>
-      </c>
-      <c r="B13" t="s">
-        <v>234</v>
       </c>
       <c r="C13" t="s">
         <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B14" t="s">
         <v>236</v>
-      </c>
-      <c r="B14" t="s">
-        <v>237</v>
       </c>
       <c r="C14" t="s">
         <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" t="s">
         <v>239</v>
-      </c>
-      <c r="B15" t="s">
-        <v>240</v>
       </c>
       <c r="C15" t="s">
         <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" t="s">
         <v>239</v>
-      </c>
-      <c r="B16" t="s">
-        <v>240</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B17" t="s">
         <v>242</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" t="s">
         <v>243</v>
-      </c>
-      <c r="C17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D17" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B18" t="s">
         <v>245</v>
-      </c>
-      <c r="B18" t="s">
-        <v>246</v>
       </c>
       <c r="C18" t="s">
         <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B19" t="s">
         <v>248</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" t="s">
         <v>249</v>
-      </c>
-      <c r="C19" t="s">
-        <v>168</v>
-      </c>
-      <c r="D19" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B20" t="s">
         <v>251</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" t="s">
         <v>252</v>
-      </c>
-      <c r="C20" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B21" t="s">
         <v>254</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" t="s">
         <v>255</v>
-      </c>
-      <c r="C21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B22" t="s">
         <v>257</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D22" t="s">
         <v>258</v>
-      </c>
-      <c r="C22" t="s">
-        <v>195</v>
-      </c>
-      <c r="D22" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B23" t="s">
         <v>260</v>
-      </c>
-      <c r="B23" t="s">
-        <v>261</v>
       </c>
       <c r="C23" t="s">
         <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B24" t="s">
         <v>263</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" t="s">
         <v>264</v>
-      </c>
-      <c r="C24" t="s">
-        <v>180</v>
-      </c>
-      <c r="D24" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B25" t="s">
         <v>266</v>
-      </c>
-      <c r="B25" t="s">
-        <v>267</v>
       </c>
       <c r="C25" t="s">
         <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26" t="s">
         <v>269</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D26" t="s">
         <v>270</v>
-      </c>
-      <c r="C26" t="s">
-        <v>185</v>
-      </c>
-      <c r="D26" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B27" t="s">
         <v>272</v>
-      </c>
-      <c r="B27" t="s">
-        <v>273</v>
       </c>
       <c r="C27" t="s">
         <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B28" t="s">
         <v>275</v>
-      </c>
-      <c r="B28" t="s">
-        <v>276</v>
       </c>
       <c r="C28" t="s">
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B29" t="s">
         <v>278</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>194</v>
+      </c>
+      <c r="D29" t="s">
         <v>279</v>
-      </c>
-      <c r="C29" t="s">
-        <v>195</v>
-      </c>
-      <c r="D29" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B30" t="s">
         <v>281</v>
-      </c>
-      <c r="B30" t="s">
-        <v>282</v>
       </c>
       <c r="C30" t="s">
         <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B31" t="s">
         <v>284</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" t="s">
         <v>285</v>
-      </c>
-      <c r="C31" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B32" t="s">
         <v>287</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" t="s">
         <v>288</v>
-      </c>
-      <c r="C32" t="s">
-        <v>163</v>
-      </c>
-      <c r="D32" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B33" t="s">
         <v>290</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>188</v>
+      </c>
+      <c r="D33" t="s">
         <v>291</v>
-      </c>
-      <c r="C33" t="s">
-        <v>189</v>
-      </c>
-      <c r="D33" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B34" t="s">
         <v>293</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>188</v>
+      </c>
+      <c r="D34" t="s">
         <v>294</v>
-      </c>
-      <c r="C34" t="s">
-        <v>189</v>
-      </c>
-      <c r="D34" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B35" t="s">
         <v>296</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>194</v>
+      </c>
+      <c r="D35" t="s">
         <v>297</v>
-      </c>
-      <c r="C35" t="s">
-        <v>195</v>
-      </c>
-      <c r="D35" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B36" t="s">
         <v>299</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>300</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>301</v>
-      </c>
-      <c r="D36" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B37" t="s">
         <v>303</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" t="s">
         <v>304</v>
-      </c>
-      <c r="C37" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B38" t="s">
         <v>306</v>
-      </c>
-      <c r="B38" t="s">
-        <v>307</v>
       </c>
       <c r="C38" t="s">
         <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="B39" t="s">
         <v>309</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" t="s">
         <v>310</v>
-      </c>
-      <c r="C39" t="s">
-        <v>172</v>
-      </c>
-      <c r="D39" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B40" t="s">
         <v>312</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" t="s">
         <v>313</v>
-      </c>
-      <c r="C40" t="s">
-        <v>114</v>
-      </c>
-      <c r="D40" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B41" t="s">
         <v>315</v>
-      </c>
-      <c r="B41" t="s">
-        <v>316</v>
       </c>
       <c r="C41" t="s">
         <v>63</v>
       </c>
       <c r="D41" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B42" t="s">
         <v>318</v>
-      </c>
-      <c r="B42" t="s">
-        <v>319</v>
       </c>
       <c r="C42" t="s">
         <v>96</v>
       </c>
       <c r="D42" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B43" t="s">
         <v>321</v>
-      </c>
-      <c r="B43" t="s">
-        <v>322</v>
       </c>
       <c r="C43" t="s">
         <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B44" t="s">
         <v>324</v>
-      </c>
-      <c r="B44" t="s">
-        <v>325</v>
       </c>
       <c r="C44" t="s">
         <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B45" t="s">
         <v>327</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
+        <v>194</v>
+      </c>
+      <c r="D45" t="s">
         <v>328</v>
-      </c>
-      <c r="C45" t="s">
-        <v>195</v>
-      </c>
-      <c r="D45" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B46" t="s">
         <v>330</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" t="s">
         <v>331</v>
-      </c>
-      <c r="C46" t="s">
-        <v>137</v>
-      </c>
-      <c r="D46" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B47" t="s">
         <v>333</v>
-      </c>
-      <c r="B47" t="s">
-        <v>334</v>
       </c>
       <c r="C47" t="s">
         <v>96</v>
       </c>
       <c r="D47" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B48" t="s">
         <v>336</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" t="s">
         <v>337</v>
-      </c>
-      <c r="C48" t="s">
-        <v>168</v>
-      </c>
-      <c r="D48" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B49" t="s">
         <v>339</v>
-      </c>
-      <c r="B49" t="s">
-        <v>340</v>
       </c>
       <c r="C49" t="s">
         <v>63</v>
       </c>
       <c r="D49" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B50" t="s">
         <v>342</v>
-      </c>
-      <c r="B50" t="s">
-        <v>343</v>
       </c>
       <c r="C50" t="s">
         <v>46</v>
       </c>
       <c r="D50" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B51" t="s">
         <v>345</v>
-      </c>
-      <c r="B51" t="s">
-        <v>346</v>
       </c>
       <c r="C51" t="s">
         <v>63</v>
       </c>
       <c r="D51" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B52" t="s">
         <v>348</v>
-      </c>
-      <c r="B52" t="s">
-        <v>349</v>
       </c>
       <c r="C52" t="s">
         <v>83</v>
       </c>
       <c r="D52" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B53" t="s">
         <v>351</v>
-      </c>
-      <c r="B53" t="s">
-        <v>352</v>
       </c>
       <c r="C53" t="s">
         <v>100</v>
       </c>
       <c r="D53" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B54" t="s">
         <v>354</v>
-      </c>
-      <c r="B54" t="s">
-        <v>355</v>
       </c>
       <c r="C54" t="s">
         <v>96</v>
       </c>
       <c r="D54" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B55" t="s">
         <v>357</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" t="s">
         <v>358</v>
-      </c>
-      <c r="C55" t="s">
-        <v>147</v>
-      </c>
-      <c r="D55" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="B56" t="s">
         <v>360</v>
-      </c>
-      <c r="B56" t="s">
-        <v>361</v>
       </c>
       <c r="C56" t="s">
         <v>28</v>
       </c>
       <c r="D56" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="B57" t="s">
         <v>363</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
+        <v>188</v>
+      </c>
+      <c r="D57" t="s">
         <v>364</v>
-      </c>
-      <c r="C57" t="s">
-        <v>189</v>
-      </c>
-      <c r="D57" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B58" t="s">
         <v>366</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
+        <v>167</v>
+      </c>
+      <c r="D58" t="s">
         <v>367</v>
-      </c>
-      <c r="C58" t="s">
-        <v>168</v>
-      </c>
-      <c r="D58" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="B59" t="s">
         <v>369</v>
-      </c>
-      <c r="B59" t="s">
-        <v>370</v>
       </c>
       <c r="C59" t="s">
         <v>88</v>
       </c>
       <c r="D59" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B60" t="s">
         <v>372</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
+        <v>188</v>
+      </c>
+      <c r="D60" t="s">
         <v>373</v>
-      </c>
-      <c r="C60" t="s">
-        <v>189</v>
-      </c>
-      <c r="D60" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B61" t="s">
         <v>375</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
+        <v>132</v>
+      </c>
+      <c r="D61" t="s">
         <v>376</v>
-      </c>
-      <c r="C61" t="s">
-        <v>133</v>
-      </c>
-      <c r="D61" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B62" t="s">
         <v>378</v>
-      </c>
-      <c r="B62" t="s">
-        <v>379</v>
       </c>
       <c r="C62" t="s">
         <v>32</v>
       </c>
       <c r="D62" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="B63" t="s">
         <v>381</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
+        <v>136</v>
+      </c>
+      <c r="D63" t="s">
         <v>382</v>
-      </c>
-      <c r="C63" t="s">
-        <v>137</v>
-      </c>
-      <c r="D63" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B64" t="s">
         <v>384</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
+        <v>171</v>
+      </c>
+      <c r="D64" t="s">
         <v>385</v>
-      </c>
-      <c r="C64" t="s">
-        <v>172</v>
-      </c>
-      <c r="D64" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="B65" t="s">
         <v>387</v>
-      </c>
-      <c r="B65" t="s">
-        <v>388</v>
       </c>
       <c r="C65" t="s">
         <v>55</v>
       </c>
       <c r="D65" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B66" t="s">
         <v>390</v>
-      </c>
-      <c r="B66" t="s">
-        <v>391</v>
       </c>
       <c r="C66" t="s">
         <v>67</v>
       </c>
       <c r="D66" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B67" t="s">
         <v>393</v>
-      </c>
-      <c r="B67" t="s">
-        <v>394</v>
       </c>
       <c r="C67" t="s">
         <v>93</v>
       </c>
       <c r="D67" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="B68" t="s">
         <v>396</v>
-      </c>
-      <c r="B68" t="s">
-        <v>397</v>
       </c>
       <c r="C68" t="s">
         <v>10</v>
       </c>
       <c r="D68" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="B69" t="s">
         <v>399</v>
-      </c>
-      <c r="B69" t="s">
-        <v>400</v>
       </c>
       <c r="C69" t="s">
         <v>104</v>
       </c>
       <c r="D69" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="B70" t="s">
         <v>402</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>140</v>
+      </c>
+      <c r="D70" t="s">
         <v>403</v>
-      </c>
-      <c r="C70" t="s">
-        <v>141</v>
-      </c>
-      <c r="D70" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B71" t="s">
         <v>405</v>
-      </c>
-      <c r="B71" t="s">
-        <v>406</v>
       </c>
       <c r="C71" t="s">
         <v>18</v>
       </c>
       <c r="D71" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B72" t="s">
         <v>408</v>
-      </c>
-      <c r="B72" t="s">
-        <v>409</v>
       </c>
       <c r="C72" t="s">
         <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B73" t="s">
         <v>411</v>
-      </c>
-      <c r="B73" t="s">
-        <v>412</v>
       </c>
       <c r="C73" t="s">
         <v>36</v>
       </c>
       <c r="D73" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B74" t="s">
         <v>414</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
+        <v>179</v>
+      </c>
+      <c r="D74" t="s">
         <v>415</v>
-      </c>
-      <c r="C74" t="s">
-        <v>180</v>
-      </c>
-      <c r="D74" t="s">
-        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -5397,7 +5369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED1E104-9062-4EAF-9E42-F22F5508C47F}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -5410,21 +5382,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B1" t="s">
         <v>417</v>
       </c>
-      <c r="B1" t="s">
-        <v>418</v>
-      </c>
       <c r="C1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B2" t="s">
         <v>419</v>
-      </c>
-      <c r="B2" t="s">
-        <v>420</v>
       </c>
       <c r="C2">
         <v>17</v>
@@ -5432,10 +5404,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B3" t="s">
         <v>421</v>
-      </c>
-      <c r="B3" t="s">
-        <v>422</v>
       </c>
       <c r="C3">
         <v>24</v>
@@ -5443,10 +5415,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B4" t="s">
         <v>423</v>
-      </c>
-      <c r="B4" t="s">
-        <v>424</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -5454,10 +5426,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B5" t="s">
         <v>425</v>
-      </c>
-      <c r="B5" t="s">
-        <v>426</v>
       </c>
       <c r="C5">
         <v>44</v>
@@ -5465,10 +5437,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>426</v>
+      </c>
+      <c r="B6" t="s">
         <v>427</v>
-      </c>
-      <c r="B6" t="s">
-        <v>428</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -5476,10 +5448,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>428</v>
+      </c>
+      <c r="B7" t="s">
         <v>429</v>
-      </c>
-      <c r="B7" t="s">
-        <v>430</v>
       </c>
       <c r="C7">
         <v>50</v>
@@ -5487,10 +5459,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>430</v>
+      </c>
+      <c r="B8" t="s">
         <v>431</v>
-      </c>
-      <c r="B8" t="s">
-        <v>432</v>
       </c>
       <c r="C8">
         <v>45</v>
@@ -5498,10 +5470,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>432</v>
+      </c>
+      <c r="B9" t="s">
         <v>433</v>
-      </c>
-      <c r="B9" t="s">
-        <v>434</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -5509,10 +5481,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>434</v>
+      </c>
+      <c r="B10" t="s">
         <v>435</v>
-      </c>
-      <c r="B10" t="s">
-        <v>436</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -5520,10 +5492,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>436</v>
+      </c>
+      <c r="B11" t="s">
         <v>437</v>
-      </c>
-      <c r="B11" t="s">
-        <v>438</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -5531,10 +5503,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>438</v>
+      </c>
+      <c r="B12" t="s">
         <v>439</v>
-      </c>
-      <c r="B12" t="s">
-        <v>440</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -5542,10 +5514,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>440</v>
+      </c>
+      <c r="B13" t="s">
         <v>441</v>
-      </c>
-      <c r="B13" t="s">
-        <v>442</v>
       </c>
       <c r="C13">
         <v>9</v>
@@ -5553,10 +5525,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>442</v>
+      </c>
+      <c r="B14" t="s">
         <v>443</v>
-      </c>
-      <c r="B14" t="s">
-        <v>444</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -5564,10 +5536,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>444</v>
+      </c>
+      <c r="B15" t="s">
         <v>445</v>
-      </c>
-      <c r="B15" t="s">
-        <v>446</v>
       </c>
       <c r="C15">
         <v>11</v>
@@ -5575,10 +5547,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>446</v>
+      </c>
+      <c r="B16" t="s">
         <v>447</v>
-      </c>
-      <c r="B16" t="s">
-        <v>448</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -5586,10 +5558,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>448</v>
+      </c>
+      <c r="B17" t="s">
         <v>449</v>
-      </c>
-      <c r="B17" t="s">
-        <v>450</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -5597,10 +5569,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>450</v>
+      </c>
+      <c r="B18" t="s">
         <v>451</v>
-      </c>
-      <c r="B18" t="s">
-        <v>452</v>
       </c>
       <c r="C18">
         <v>13</v>
@@ -5608,10 +5580,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>452</v>
+      </c>
+      <c r="B19" t="s">
         <v>453</v>
-      </c>
-      <c r="B19" t="s">
-        <v>454</v>
       </c>
       <c r="C19">
         <v>15</v>
@@ -5619,10 +5591,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>454</v>
+      </c>
+      <c r="B20" t="s">
         <v>455</v>
-      </c>
-      <c r="B20" t="s">
-        <v>456</v>
       </c>
       <c r="C20">
         <v>16</v>
@@ -5630,10 +5602,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>456</v>
+      </c>
+      <c r="B21" t="s">
         <v>457</v>
-      </c>
-      <c r="B21" t="s">
-        <v>458</v>
       </c>
       <c r="C21">
         <v>46</v>
@@ -5641,10 +5613,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>458</v>
+      </c>
+      <c r="B22" t="s">
         <v>459</v>
-      </c>
-      <c r="B22" t="s">
-        <v>460</v>
       </c>
       <c r="C22">
         <v>57</v>
@@ -5652,10 +5624,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>460</v>
+      </c>
+      <c r="B23" t="s">
         <v>461</v>
-      </c>
-      <c r="B23" t="s">
-        <v>462</v>
       </c>
       <c r="C23">
         <v>33</v>
@@ -5663,10 +5635,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>462</v>
+      </c>
+      <c r="B24" t="s">
         <v>463</v>
-      </c>
-      <c r="B24" t="s">
-        <v>464</v>
       </c>
       <c r="C24">
         <v>18</v>
@@ -5674,10 +5646,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>464</v>
+      </c>
+      <c r="B25" t="s">
         <v>465</v>
-      </c>
-      <c r="B25" t="s">
-        <v>466</v>
       </c>
       <c r="C25">
         <v>19</v>
@@ -5685,10 +5657,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>466</v>
+      </c>
+      <c r="B26" t="s">
         <v>467</v>
-      </c>
-      <c r="B26" t="s">
-        <v>468</v>
       </c>
       <c r="C26">
         <v>20</v>
@@ -5696,10 +5668,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>468</v>
+      </c>
+      <c r="B27" t="s">
         <v>469</v>
-      </c>
-      <c r="B27" t="s">
-        <v>470</v>
       </c>
       <c r="C27">
         <v>21</v>
@@ -5707,10 +5679,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>470</v>
+      </c>
+      <c r="B28" t="s">
         <v>471</v>
-      </c>
-      <c r="B28" t="s">
-        <v>472</v>
       </c>
       <c r="C28">
         <v>14</v>
@@ -5718,10 +5690,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>472</v>
+      </c>
+      <c r="B29" t="s">
         <v>473</v>
-      </c>
-      <c r="B29" t="s">
-        <v>474</v>
       </c>
       <c r="C29">
         <v>22</v>
@@ -5729,10 +5701,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C30">
         <v>23</v>
@@ -5740,10 +5712,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>475</v>
+      </c>
+      <c r="B31" t="s">
         <v>476</v>
-      </c>
-      <c r="B31" t="s">
-        <v>477</v>
       </c>
       <c r="C31">
         <v>26</v>
@@ -5751,10 +5723,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>477</v>
+      </c>
+      <c r="B32" t="s">
         <v>478</v>
-      </c>
-      <c r="B32" t="s">
-        <v>479</v>
       </c>
       <c r="C32">
         <v>27</v>
@@ -5762,10 +5734,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>479</v>
+      </c>
+      <c r="B33" t="s">
         <v>480</v>
-      </c>
-      <c r="B33" t="s">
-        <v>481</v>
       </c>
       <c r="C33">
         <v>28</v>
@@ -5773,10 +5745,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>481</v>
+      </c>
+      <c r="B34" t="s">
         <v>482</v>
-      </c>
-      <c r="B34" t="s">
-        <v>483</v>
       </c>
       <c r="C34">
         <v>56</v>
@@ -5784,10 +5756,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>483</v>
+      </c>
+      <c r="B35" t="s">
         <v>484</v>
-      </c>
-      <c r="B35" t="s">
-        <v>485</v>
       </c>
       <c r="C35">
         <v>29</v>
@@ -5795,10 +5767,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>485</v>
+      </c>
+      <c r="B36" t="s">
         <v>486</v>
-      </c>
-      <c r="B36" t="s">
-        <v>487</v>
       </c>
       <c r="C36">
         <v>39</v>
@@ -5806,10 +5778,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>487</v>
+      </c>
+      <c r="B37" t="s">
         <v>488</v>
-      </c>
-      <c r="B37" t="s">
-        <v>489</v>
       </c>
       <c r="C37">
         <v>30</v>
@@ -5817,10 +5789,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>489</v>
+      </c>
+      <c r="B38" t="s">
         <v>490</v>
-      </c>
-      <c r="B38" t="s">
-        <v>491</v>
       </c>
       <c r="C38">
         <v>53</v>
@@ -5828,10 +5800,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>491</v>
+      </c>
+      <c r="B39" t="s">
         <v>492</v>
-      </c>
-      <c r="B39" t="s">
-        <v>493</v>
       </c>
       <c r="C39">
         <v>5</v>
@@ -5839,10 +5811,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>493</v>
+      </c>
+      <c r="B40" t="s">
         <v>494</v>
-      </c>
-      <c r="B40" t="s">
-        <v>495</v>
       </c>
       <c r="C40">
         <v>31</v>
@@ -5850,10 +5822,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>495</v>
+      </c>
+      <c r="B41" t="s">
         <v>496</v>
-      </c>
-      <c r="B41" t="s">
-        <v>497</v>
       </c>
       <c r="C41">
         <v>32</v>
@@ -5861,10 +5833,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>497</v>
+      </c>
+      <c r="B42" t="s">
         <v>498</v>
-      </c>
-      <c r="B42" t="s">
-        <v>499</v>
       </c>
       <c r="C42">
         <v>42</v>

</xml_diff>

<commit_message>
corrected st daio and dai rank calculation
</commit_message>
<xml_diff>
--- a/stakeholder_lists.xlsx
+++ b/stakeholder_lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\mobile-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343AF638-C776-4EE9-9D0A-E9258E5822B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599CD7AE-C7CD-4727-B34D-5D41253E533C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{17D0CF8C-6239-4396-93EE-ED3916C7EA4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="2" xr2:uid="{17D0CF8C-6239-4396-93EE-ED3916C7EA4B}"/>
   </bookViews>
   <sheets>
     <sheet name="state_lists" sheetId="1" r:id="rId1"/>
@@ -1462,9 +1462,6 @@
     <t>MOLDATSA</t>
   </si>
   <si>
-    <t>MAS_ANSP</t>
-  </si>
-  <si>
     <t>GB_ANSP</t>
   </si>
   <si>
@@ -1538,6 +1535,9 @@
   </si>
   <si>
     <t>ANSP_ID</t>
+  </si>
+  <si>
+    <t>MUAC_ANSP</t>
   </si>
 </sst>
 </file>
@@ -2119,7 +2119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504966A5-1D6A-4873-89C5-14DFD4258010}">
   <dimension ref="B2:Z47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="X27" sqref="X27:Z27"/>
     </sheetView>
   </sheetViews>
@@ -5369,8 +5369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED1E104-9062-4EAF-9E42-F22F5508C47F}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5388,7 +5388,7 @@
         <v>417</v>
       </c>
       <c r="C1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5701,7 +5701,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>474</v>
+        <v>499</v>
       </c>
       <c r="B30" t="s">
         <v>111</v>
@@ -5712,10 +5712,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>474</v>
+      </c>
+      <c r="B31" t="s">
         <v>475</v>
-      </c>
-      <c r="B31" t="s">
-        <v>476</v>
       </c>
       <c r="C31">
         <v>26</v>
@@ -5723,10 +5723,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>476</v>
+      </c>
+      <c r="B32" t="s">
         <v>477</v>
-      </c>
-      <c r="B32" t="s">
-        <v>478</v>
       </c>
       <c r="C32">
         <v>27</v>
@@ -5734,10 +5734,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>478</v>
+      </c>
+      <c r="B33" t="s">
         <v>479</v>
-      </c>
-      <c r="B33" t="s">
-        <v>480</v>
       </c>
       <c r="C33">
         <v>28</v>
@@ -5745,10 +5745,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>480</v>
+      </c>
+      <c r="B34" t="s">
         <v>481</v>
-      </c>
-      <c r="B34" t="s">
-        <v>482</v>
       </c>
       <c r="C34">
         <v>56</v>
@@ -5756,10 +5756,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>482</v>
+      </c>
+      <c r="B35" t="s">
         <v>483</v>
-      </c>
-      <c r="B35" t="s">
-        <v>484</v>
       </c>
       <c r="C35">
         <v>29</v>
@@ -5767,10 +5767,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>484</v>
+      </c>
+      <c r="B36" t="s">
         <v>485</v>
-      </c>
-      <c r="B36" t="s">
-        <v>486</v>
       </c>
       <c r="C36">
         <v>39</v>
@@ -5778,10 +5778,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>486</v>
+      </c>
+      <c r="B37" t="s">
         <v>487</v>
-      </c>
-      <c r="B37" t="s">
-        <v>488</v>
       </c>
       <c r="C37">
         <v>30</v>
@@ -5789,10 +5789,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>488</v>
+      </c>
+      <c r="B38" t="s">
         <v>489</v>
-      </c>
-      <c r="B38" t="s">
-        <v>490</v>
       </c>
       <c r="C38">
         <v>53</v>
@@ -5800,10 +5800,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>490</v>
+      </c>
+      <c r="B39" t="s">
         <v>491</v>
-      </c>
-      <c r="B39" t="s">
-        <v>492</v>
       </c>
       <c r="C39">
         <v>5</v>
@@ -5811,10 +5811,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>492</v>
+      </c>
+      <c r="B40" t="s">
         <v>493</v>
-      </c>
-      <c r="B40" t="s">
-        <v>494</v>
       </c>
       <c r="C40">
         <v>31</v>
@@ -5822,10 +5822,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>494</v>
+      </c>
+      <c r="B41" t="s">
         <v>495</v>
-      </c>
-      <c r="B41" t="s">
-        <v>496</v>
       </c>
       <c r="C41">
         <v>32</v>
@@ -5833,10 +5833,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>496</v>
+      </c>
+      <c r="B42" t="s">
         <v>497</v>
-      </c>
-      <c r="B42" t="s">
-        <v>498</v>
       </c>
       <c r="C42">
         <v>42</v>

</xml_diff>

<commit_message>
adjusted acc name for muac
</commit_message>
<xml_diff>
--- a/stakeholder_lists.xlsx
+++ b/stakeholder_lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\mobile-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599CD7AE-C7CD-4727-B34D-5D41253E533C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607F7AEC-318F-4D1B-BBA7-187491980C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="2" xr2:uid="{17D0CF8C-6239-4396-93EE-ED3916C7EA4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="1" xr2:uid="{17D0CF8C-6239-4396-93EE-ED3916C7EA4B}"/>
   </bookViews>
   <sheets>
     <sheet name="state_lists" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="499">
   <si>
     <t>state</t>
   </si>
@@ -938,9 +938,6 @@
   </si>
   <si>
     <t>Maastricht UAC</t>
-  </si>
-  <si>
-    <t>MAS</t>
   </si>
   <si>
     <t>EDYYUAC</t>
@@ -4309,8 +4306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE1B1DA-244C-4D7E-AA08-285D46CCB17C}">
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4819,542 +4816,542 @@
         <v>299</v>
       </c>
       <c r="C36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" t="s">
         <v>300</v>
-      </c>
-      <c r="D36" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B37" t="s">
         <v>302</v>
-      </c>
-      <c r="B37" t="s">
-        <v>303</v>
       </c>
       <c r="C37" t="s">
         <v>167</v>
       </c>
       <c r="D37" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B38" t="s">
         <v>305</v>
-      </c>
-      <c r="B38" t="s">
-        <v>306</v>
       </c>
       <c r="C38" t="s">
         <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B39" t="s">
         <v>308</v>
-      </c>
-      <c r="B39" t="s">
-        <v>309</v>
       </c>
       <c r="C39" t="s">
         <v>171</v>
       </c>
       <c r="D39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B40" t="s">
         <v>311</v>
-      </c>
-      <c r="B40" t="s">
-        <v>312</v>
       </c>
       <c r="C40" t="s">
         <v>113</v>
       </c>
       <c r="D40" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B41" t="s">
         <v>314</v>
-      </c>
-      <c r="B41" t="s">
-        <v>315</v>
       </c>
       <c r="C41" t="s">
         <v>63</v>
       </c>
       <c r="D41" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B42" t="s">
         <v>317</v>
-      </c>
-      <c r="B42" t="s">
-        <v>318</v>
       </c>
       <c r="C42" t="s">
         <v>96</v>
       </c>
       <c r="D42" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B43" t="s">
         <v>320</v>
-      </c>
-      <c r="B43" t="s">
-        <v>321</v>
       </c>
       <c r="C43" t="s">
         <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B44" t="s">
         <v>323</v>
-      </c>
-      <c r="B44" t="s">
-        <v>324</v>
       </c>
       <c r="C44" t="s">
         <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B45" t="s">
         <v>326</v>
-      </c>
-      <c r="B45" t="s">
-        <v>327</v>
       </c>
       <c r="C45" t="s">
         <v>194</v>
       </c>
       <c r="D45" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B46" t="s">
         <v>329</v>
-      </c>
-      <c r="B46" t="s">
-        <v>330</v>
       </c>
       <c r="C46" t="s">
         <v>136</v>
       </c>
       <c r="D46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B47" t="s">
         <v>332</v>
-      </c>
-      <c r="B47" t="s">
-        <v>333</v>
       </c>
       <c r="C47" t="s">
         <v>96</v>
       </c>
       <c r="D47" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B48" t="s">
         <v>335</v>
-      </c>
-      <c r="B48" t="s">
-        <v>336</v>
       </c>
       <c r="C48" t="s">
         <v>167</v>
       </c>
       <c r="D48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B49" t="s">
         <v>338</v>
-      </c>
-      <c r="B49" t="s">
-        <v>339</v>
       </c>
       <c r="C49" t="s">
         <v>63</v>
       </c>
       <c r="D49" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B50" t="s">
         <v>341</v>
-      </c>
-      <c r="B50" t="s">
-        <v>342</v>
       </c>
       <c r="C50" t="s">
         <v>46</v>
       </c>
       <c r="D50" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B51" t="s">
         <v>344</v>
-      </c>
-      <c r="B51" t="s">
-        <v>345</v>
       </c>
       <c r="C51" t="s">
         <v>63</v>
       </c>
       <c r="D51" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B52" t="s">
         <v>347</v>
-      </c>
-      <c r="B52" t="s">
-        <v>348</v>
       </c>
       <c r="C52" t="s">
         <v>83</v>
       </c>
       <c r="D52" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B53" t="s">
         <v>350</v>
-      </c>
-      <c r="B53" t="s">
-        <v>351</v>
       </c>
       <c r="C53" t="s">
         <v>100</v>
       </c>
       <c r="D53" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B54" t="s">
         <v>353</v>
-      </c>
-      <c r="B54" t="s">
-        <v>354</v>
       </c>
       <c r="C54" t="s">
         <v>96</v>
       </c>
       <c r="D54" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B55" t="s">
         <v>356</v>
-      </c>
-      <c r="B55" t="s">
-        <v>357</v>
       </c>
       <c r="C55" t="s">
         <v>146</v>
       </c>
       <c r="D55" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="B56" t="s">
         <v>359</v>
-      </c>
-      <c r="B56" t="s">
-        <v>360</v>
       </c>
       <c r="C56" t="s">
         <v>28</v>
       </c>
       <c r="D56" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B57" t="s">
         <v>362</v>
-      </c>
-      <c r="B57" t="s">
-        <v>363</v>
       </c>
       <c r="C57" t="s">
         <v>188</v>
       </c>
       <c r="D57" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="B58" t="s">
         <v>365</v>
-      </c>
-      <c r="B58" t="s">
-        <v>366</v>
       </c>
       <c r="C58" t="s">
         <v>167</v>
       </c>
       <c r="D58" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B59" t="s">
         <v>368</v>
-      </c>
-      <c r="B59" t="s">
-        <v>369</v>
       </c>
       <c r="C59" t="s">
         <v>88</v>
       </c>
       <c r="D59" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B60" t="s">
         <v>371</v>
-      </c>
-      <c r="B60" t="s">
-        <v>372</v>
       </c>
       <c r="C60" t="s">
         <v>188</v>
       </c>
       <c r="D60" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B61" t="s">
         <v>374</v>
-      </c>
-      <c r="B61" t="s">
-        <v>375</v>
       </c>
       <c r="C61" t="s">
         <v>132</v>
       </c>
       <c r="D61" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B62" t="s">
         <v>377</v>
-      </c>
-      <c r="B62" t="s">
-        <v>378</v>
       </c>
       <c r="C62" t="s">
         <v>32</v>
       </c>
       <c r="D62" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B63" t="s">
         <v>380</v>
-      </c>
-      <c r="B63" t="s">
-        <v>381</v>
       </c>
       <c r="C63" t="s">
         <v>136</v>
       </c>
       <c r="D63" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B64" t="s">
         <v>383</v>
-      </c>
-      <c r="B64" t="s">
-        <v>384</v>
       </c>
       <c r="C64" t="s">
         <v>171</v>
       </c>
       <c r="D64" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B65" t="s">
         <v>386</v>
-      </c>
-      <c r="B65" t="s">
-        <v>387</v>
       </c>
       <c r="C65" t="s">
         <v>55</v>
       </c>
       <c r="D65" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="B66" t="s">
         <v>389</v>
-      </c>
-      <c r="B66" t="s">
-        <v>390</v>
       </c>
       <c r="C66" t="s">
         <v>67</v>
       </c>
       <c r="D66" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="B67" t="s">
         <v>392</v>
-      </c>
-      <c r="B67" t="s">
-        <v>393</v>
       </c>
       <c r="C67" t="s">
         <v>93</v>
       </c>
       <c r="D67" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="B68" t="s">
         <v>395</v>
-      </c>
-      <c r="B68" t="s">
-        <v>396</v>
       </c>
       <c r="C68" t="s">
         <v>10</v>
       </c>
       <c r="D68" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="B69" t="s">
         <v>398</v>
-      </c>
-      <c r="B69" t="s">
-        <v>399</v>
       </c>
       <c r="C69" t="s">
         <v>104</v>
       </c>
       <c r="D69" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="B70" t="s">
         <v>401</v>
-      </c>
-      <c r="B70" t="s">
-        <v>402</v>
       </c>
       <c r="C70" t="s">
         <v>140</v>
       </c>
       <c r="D70" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="B71" t="s">
         <v>404</v>
-      </c>
-      <c r="B71" t="s">
-        <v>405</v>
       </c>
       <c r="C71" t="s">
         <v>18</v>
       </c>
       <c r="D71" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="B72" t="s">
         <v>407</v>
-      </c>
-      <c r="B72" t="s">
-        <v>408</v>
       </c>
       <c r="C72" t="s">
         <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B73" t="s">
         <v>410</v>
-      </c>
-      <c r="B73" t="s">
-        <v>411</v>
       </c>
       <c r="C73" t="s">
         <v>36</v>
       </c>
       <c r="D73" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="B74" t="s">
         <v>413</v>
-      </c>
-      <c r="B74" t="s">
-        <v>414</v>
       </c>
       <c r="C74" t="s">
         <v>179</v>
       </c>
       <c r="D74" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -5369,7 +5366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED1E104-9062-4EAF-9E42-F22F5508C47F}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -5382,21 +5379,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B1" t="s">
         <v>416</v>
       </c>
-      <c r="B1" t="s">
-        <v>417</v>
-      </c>
       <c r="C1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" t="s">
         <v>418</v>
-      </c>
-      <c r="B2" t="s">
-        <v>419</v>
       </c>
       <c r="C2">
         <v>17</v>
@@ -5404,10 +5401,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B3" t="s">
         <v>420</v>
-      </c>
-      <c r="B3" t="s">
-        <v>421</v>
       </c>
       <c r="C3">
         <v>24</v>
@@ -5415,10 +5412,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>421</v>
+      </c>
+      <c r="B4" t="s">
         <v>422</v>
-      </c>
-      <c r="B4" t="s">
-        <v>423</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -5426,10 +5423,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B5" t="s">
         <v>424</v>
-      </c>
-      <c r="B5" t="s">
-        <v>425</v>
       </c>
       <c r="C5">
         <v>44</v>
@@ -5437,10 +5434,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>425</v>
+      </c>
+      <c r="B6" t="s">
         <v>426</v>
-      </c>
-      <c r="B6" t="s">
-        <v>427</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -5448,10 +5445,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>427</v>
+      </c>
+      <c r="B7" t="s">
         <v>428</v>
-      </c>
-      <c r="B7" t="s">
-        <v>429</v>
       </c>
       <c r="C7">
         <v>50</v>
@@ -5459,10 +5456,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B8" t="s">
         <v>430</v>
-      </c>
-      <c r="B8" t="s">
-        <v>431</v>
       </c>
       <c r="C8">
         <v>45</v>
@@ -5470,10 +5467,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>431</v>
+      </c>
+      <c r="B9" t="s">
         <v>432</v>
-      </c>
-      <c r="B9" t="s">
-        <v>433</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -5481,10 +5478,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>433</v>
+      </c>
+      <c r="B10" t="s">
         <v>434</v>
-      </c>
-      <c r="B10" t="s">
-        <v>435</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -5492,10 +5489,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>435</v>
+      </c>
+      <c r="B11" t="s">
         <v>436</v>
-      </c>
-      <c r="B11" t="s">
-        <v>437</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -5503,10 +5500,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>437</v>
+      </c>
+      <c r="B12" t="s">
         <v>438</v>
-      </c>
-      <c r="B12" t="s">
-        <v>439</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -5514,10 +5511,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>439</v>
+      </c>
+      <c r="B13" t="s">
         <v>440</v>
-      </c>
-      <c r="B13" t="s">
-        <v>441</v>
       </c>
       <c r="C13">
         <v>9</v>
@@ -5525,10 +5522,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>441</v>
+      </c>
+      <c r="B14" t="s">
         <v>442</v>
-      </c>
-      <c r="B14" t="s">
-        <v>443</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -5536,10 +5533,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>443</v>
+      </c>
+      <c r="B15" t="s">
         <v>444</v>
-      </c>
-      <c r="B15" t="s">
-        <v>445</v>
       </c>
       <c r="C15">
         <v>11</v>
@@ -5547,10 +5544,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>445</v>
+      </c>
+      <c r="B16" t="s">
         <v>446</v>
-      </c>
-      <c r="B16" t="s">
-        <v>447</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -5558,10 +5555,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>447</v>
+      </c>
+      <c r="B17" t="s">
         <v>448</v>
-      </c>
-      <c r="B17" t="s">
-        <v>449</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -5569,10 +5566,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>449</v>
+      </c>
+      <c r="B18" t="s">
         <v>450</v>
-      </c>
-      <c r="B18" t="s">
-        <v>451</v>
       </c>
       <c r="C18">
         <v>13</v>
@@ -5580,10 +5577,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>451</v>
+      </c>
+      <c r="B19" t="s">
         <v>452</v>
-      </c>
-      <c r="B19" t="s">
-        <v>453</v>
       </c>
       <c r="C19">
         <v>15</v>
@@ -5591,10 +5588,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>453</v>
+      </c>
+      <c r="B20" t="s">
         <v>454</v>
-      </c>
-      <c r="B20" t="s">
-        <v>455</v>
       </c>
       <c r="C20">
         <v>16</v>
@@ -5602,10 +5599,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>455</v>
+      </c>
+      <c r="B21" t="s">
         <v>456</v>
-      </c>
-      <c r="B21" t="s">
-        <v>457</v>
       </c>
       <c r="C21">
         <v>46</v>
@@ -5613,10 +5610,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>457</v>
+      </c>
+      <c r="B22" t="s">
         <v>458</v>
-      </c>
-      <c r="B22" t="s">
-        <v>459</v>
       </c>
       <c r="C22">
         <v>57</v>
@@ -5624,10 +5621,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>459</v>
+      </c>
+      <c r="B23" t="s">
         <v>460</v>
-      </c>
-      <c r="B23" t="s">
-        <v>461</v>
       </c>
       <c r="C23">
         <v>33</v>
@@ -5635,10 +5632,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>461</v>
+      </c>
+      <c r="B24" t="s">
         <v>462</v>
-      </c>
-      <c r="B24" t="s">
-        <v>463</v>
       </c>
       <c r="C24">
         <v>18</v>
@@ -5646,10 +5643,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>463</v>
+      </c>
+      <c r="B25" t="s">
         <v>464</v>
-      </c>
-      <c r="B25" t="s">
-        <v>465</v>
       </c>
       <c r="C25">
         <v>19</v>
@@ -5657,10 +5654,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>465</v>
+      </c>
+      <c r="B26" t="s">
         <v>466</v>
-      </c>
-      <c r="B26" t="s">
-        <v>467</v>
       </c>
       <c r="C26">
         <v>20</v>
@@ -5668,10 +5665,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>467</v>
+      </c>
+      <c r="B27" t="s">
         <v>468</v>
-      </c>
-      <c r="B27" t="s">
-        <v>469</v>
       </c>
       <c r="C27">
         <v>21</v>
@@ -5679,10 +5676,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>469</v>
+      </c>
+      <c r="B28" t="s">
         <v>470</v>
-      </c>
-      <c r="B28" t="s">
-        <v>471</v>
       </c>
       <c r="C28">
         <v>14</v>
@@ -5690,10 +5687,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>471</v>
+      </c>
+      <c r="B29" t="s">
         <v>472</v>
-      </c>
-      <c r="B29" t="s">
-        <v>473</v>
       </c>
       <c r="C29">
         <v>22</v>
@@ -5701,7 +5698,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B30" t="s">
         <v>111</v>
@@ -5712,10 +5709,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>473</v>
+      </c>
+      <c r="B31" t="s">
         <v>474</v>
-      </c>
-      <c r="B31" t="s">
-        <v>475</v>
       </c>
       <c r="C31">
         <v>26</v>
@@ -5723,10 +5720,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>475</v>
+      </c>
+      <c r="B32" t="s">
         <v>476</v>
-      </c>
-      <c r="B32" t="s">
-        <v>477</v>
       </c>
       <c r="C32">
         <v>27</v>
@@ -5734,10 +5731,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>477</v>
+      </c>
+      <c r="B33" t="s">
         <v>478</v>
-      </c>
-      <c r="B33" t="s">
-        <v>479</v>
       </c>
       <c r="C33">
         <v>28</v>
@@ -5745,10 +5742,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>479</v>
+      </c>
+      <c r="B34" t="s">
         <v>480</v>
-      </c>
-      <c r="B34" t="s">
-        <v>481</v>
       </c>
       <c r="C34">
         <v>56</v>
@@ -5756,10 +5753,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>481</v>
+      </c>
+      <c r="B35" t="s">
         <v>482</v>
-      </c>
-      <c r="B35" t="s">
-        <v>483</v>
       </c>
       <c r="C35">
         <v>29</v>
@@ -5767,10 +5764,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>483</v>
+      </c>
+      <c r="B36" t="s">
         <v>484</v>
-      </c>
-      <c r="B36" t="s">
-        <v>485</v>
       </c>
       <c r="C36">
         <v>39</v>
@@ -5778,10 +5775,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>485</v>
+      </c>
+      <c r="B37" t="s">
         <v>486</v>
-      </c>
-      <c r="B37" t="s">
-        <v>487</v>
       </c>
       <c r="C37">
         <v>30</v>
@@ -5789,10 +5786,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>487</v>
+      </c>
+      <c r="B38" t="s">
         <v>488</v>
-      </c>
-      <c r="B38" t="s">
-        <v>489</v>
       </c>
       <c r="C38">
         <v>53</v>
@@ -5800,10 +5797,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>489</v>
+      </c>
+      <c r="B39" t="s">
         <v>490</v>
-      </c>
-      <c r="B39" t="s">
-        <v>491</v>
       </c>
       <c r="C39">
         <v>5</v>
@@ -5811,10 +5808,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>491</v>
+      </c>
+      <c r="B40" t="s">
         <v>492</v>
-      </c>
-      <c r="B40" t="s">
-        <v>493</v>
       </c>
       <c r="C40">
         <v>31</v>
@@ -5822,10 +5819,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>493</v>
+      </c>
+      <c r="B41" t="s">
         <v>494</v>
-      </c>
-      <c r="B41" t="s">
-        <v>495</v>
       </c>
       <c r="C41">
         <v>32</v>
@@ -5833,10 +5830,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>495</v>
+      </c>
+      <c r="B42" t="s">
         <v>496</v>
-      </c>
-      <c r="B42" t="s">
-        <v>497</v>
       </c>
       <c r="C42">
         <v>42</v>

</xml_diff>